<commit_message>
Console Baggage System small changes
</commit_message>
<xml_diff>
--- a/ThreadSync/ThreadSync_BaggageHandlingSystem/BaggageHandlingSystem/bin/Debug/ReservationGenerator.xlsx
+++ b/ThreadSync/ThreadSync_BaggageHandlingSystem/BaggageHandlingSystem/bin/Debug/ReservationGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjedt\source\repos_git\_SchoolWork\ThreadSync\ThreadSync_BaggageHandlingSystem\BaggageHandlingSystem\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EE1E25-9220-4899-A7BA-E2C11CA119EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11A1A59-0912-48AC-91DA-BB9CFACB6B2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31635" yWindow="4140" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{9C29B736-50C8-4AEB-AA05-EAA881D5DAC3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9C29B736-50C8-4AEB-AA05-EAA881D5DAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy\ hh:mm:ss;@"/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yy\ hh:mm:ss;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy\ hh:mm:ss;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -436,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,7 +754,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,11 +785,11 @@
       </c>
       <c r="C2" s="1">
         <f ca="1">NOW()+2/24/60</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">C2+3/24/60</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -801,11 +801,11 @@
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C4" ca="1" si="0">NOW()+2/24/60</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="D3" s="1">
         <f ca="1">C3+5/24/60</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,11 +817,11 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="D4" s="1">
         <f ca="1">C4+4/24/60</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -833,11 +833,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">D2+2/24/60</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">C5+4/24/60</f>
-        <v>44260.629666898145</v>
+        <v>44263.763417013884</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -849,11 +849,11 @@
       </c>
       <c r="C6" s="1">
         <f ca="1">D3+1/24/60</f>
-        <v>44260.627583564812</v>
+        <v>44263.761333680552</v>
       </c>
       <c r="D6" s="1">
         <f ca="1">C6+3/24/60</f>
-        <v>44260.629666898145</v>
+        <v>44263.763417013884</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -865,11 +865,11 @@
       </c>
       <c r="C7" s="1">
         <f ca="1">D4+2/24/60</f>
-        <v>44260.627583564812</v>
+        <v>44263.761333680552</v>
       </c>
       <c r="D7" s="1">
         <f ca="1">C7+5/24/60</f>
-        <v>44260.631055787031</v>
+        <v>44263.764805902771</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F013B4FB-C891-40D9-903B-3DAA8FC8D684}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,11 +941,11 @@
       </c>
       <c r="E2" s="3" cm="1">
         <f t="array" aca="1" ref="E2" ca="1">_xlfn.IFS(D2=1,'Ark1'!$C$2,D2=2, 'Ark1'!$C$3,D2=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F2" s="3" cm="1">
         <f t="array" aca="1" ref="F2" ca="1">_xlfn.IFS(D2=1,'Ark1'!$D$2,D2=2, 'Ark1'!$D$3,D2=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -957,19 +957,19 @@
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">_xlfn.IFS(D3=1,"CPH",D3=2, "LON",D3=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" cm="1">
         <f t="array" aca="1" ref="E3" ca="1">_xlfn.IFS(D3=1,'Ark1'!$C$2,D3=2, 'Ark1'!$C$3,D3=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F3" s="3" cm="1">
         <f t="array" aca="1" ref="F3" ca="1">_xlfn.IFS(D3=1,'Ark1'!$D$2,D3=2, 'Ark1'!$D$3,D3=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -981,19 +981,19 @@
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">_xlfn.IFS(D4=1,"CPH",D4=2, "LON",D4=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D66" ca="1" si="0">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3" cm="1">
         <f t="array" aca="1" ref="E4" ca="1">_xlfn.IFS(D4=1,'Ark1'!$C$2,D4=2, 'Ark1'!$C$3,D4=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F4" s="3" cm="1">
         <f t="array" aca="1" ref="F4" ca="1">_xlfn.IFS(D4=1,'Ark1'!$D$2,D4=2, 'Ark1'!$D$3,D4=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1005,19 +1005,19 @@
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xlfn.IFS(D5=1,"CPH",D5=2, "LON",D5=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="3" cm="1">
         <f t="array" aca="1" ref="E5" ca="1">_xlfn.IFS(D5=1,'Ark1'!$C$2,D5=2, 'Ark1'!$C$3,D5=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F5" s="3" cm="1">
         <f t="array" aca="1" ref="F5" ca="1">_xlfn.IFS(D5=1,'Ark1'!$D$2,D5=2, 'Ark1'!$D$3,D5=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1037,11 +1037,11 @@
       </c>
       <c r="E6" s="3" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">_xlfn.IFS(D6=1,'Ark1'!$C$2,D6=2, 'Ark1'!$C$3,D6=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F6" s="3" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">_xlfn.IFS(D6=1,'Ark1'!$D$2,D6=2, 'Ark1'!$D$3,D6=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1053,19 +1053,19 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xlfn.IFS(D7=1,"CPH",D7=2, "LON",D7=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_xlfn.IFS(D7=1,'Ark1'!$C$2,D7=2, 'Ark1'!$C$3,D7=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F7" s="3" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">_xlfn.IFS(D7=1,'Ark1'!$D$2,D7=2, 'Ark1'!$D$3,D7=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1077,19 +1077,19 @@
       </c>
       <c r="C8" t="str" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xlfn.IFS(D8=1,"CPH",D8=2, "LON",D8=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">_xlfn.IFS(D8=1,'Ark1'!$C$2,D8=2, 'Ark1'!$C$3,D8=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F8" s="3" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">_xlfn.IFS(D8=1,'Ark1'!$D$2,D8=2, 'Ark1'!$D$3,D8=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1101,19 +1101,19 @@
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">_xlfn.IFS(D9=1,"CPH",D9=2, "LON",D9=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xlfn.IFS(D9=1,'Ark1'!$C$2,D9=2, 'Ark1'!$C$3,D9=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F9" s="3" cm="1">
         <f t="array" aca="1" ref="F9" ca="1">_xlfn.IFS(D9=1,'Ark1'!$D$2,D9=2, 'Ark1'!$D$3,D9=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1133,11 +1133,11 @@
       </c>
       <c r="E10" s="3" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">_xlfn.IFS(D10=1,'Ark1'!$C$2,D10=2, 'Ark1'!$C$3,D10=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F10" s="3" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">_xlfn.IFS(D10=1,'Ark1'!$D$2,D10=2, 'Ark1'!$D$3,D10=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1149,19 +1149,19 @@
       </c>
       <c r="C11" t="str" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">_xlfn.IFS(D11=1,"CPH",D11=2, "LON",D11=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">_xlfn.IFS(D11=1,'Ark1'!$C$2,D11=2, 'Ark1'!$C$3,D11=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F11" s="3" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">_xlfn.IFS(D11=1,'Ark1'!$D$2,D11=2, 'Ark1'!$D$3,D11=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1173,19 +1173,19 @@
       </c>
       <c r="C12" t="str" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_xlfn.IFS(D12=1,"CPH",D12=2, "LON",D12=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3" cm="1">
         <f t="array" aca="1" ref="E12" ca="1">_xlfn.IFS(D12=1,'Ark1'!$C$2,D12=2, 'Ark1'!$C$3,D12=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F12" s="3" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">_xlfn.IFS(D12=1,'Ark1'!$D$2,D12=2, 'Ark1'!$D$3,D12=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1205,11 +1205,11 @@
       </c>
       <c r="E13" s="3" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">_xlfn.IFS(D13=1,'Ark1'!$C$2,D13=2, 'Ark1'!$C$3,D13=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F13" s="3" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">_xlfn.IFS(D13=1,'Ark1'!$D$2,D13=2, 'Ark1'!$D$3,D13=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1221,19 +1221,19 @@
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">_xlfn.IFS(D14=1,"CPH",D14=2, "LON",D14=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f ca="1">RANDBETWEEN(1,3)</f>
+        <v>2</v>
       </c>
       <c r="E14" s="3" cm="1">
         <f t="array" aca="1" ref="E14" ca="1">_xlfn.IFS(D14=1,'Ark1'!$C$2,D14=2, 'Ark1'!$C$3,D14=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F14" s="3" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">_xlfn.IFS(D14=1,'Ark1'!$D$2,D14=2, 'Ark1'!$D$3,D14=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1245,19 +1245,19 @@
       </c>
       <c r="C15" t="str" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">_xlfn.IFS(D15=1,"CPH",D15=2, "LON",D15=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="3" cm="1">
         <f t="array" aca="1" ref="E15" ca="1">_xlfn.IFS(D15=1,'Ark1'!$C$2,D15=2, 'Ark1'!$C$3,D15=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F15" s="3" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">_xlfn.IFS(D15=1,'Ark1'!$D$2,D15=2, 'Ark1'!$D$3,D15=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1277,11 +1277,11 @@
       </c>
       <c r="E16" s="3" cm="1">
         <f t="array" aca="1" ref="E16" ca="1">_xlfn.IFS(D16=1,'Ark1'!$C$2,D16=2, 'Ark1'!$C$3,D16=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F16" s="3" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">_xlfn.IFS(D16=1,'Ark1'!$D$2,D16=2, 'Ark1'!$D$3,D16=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,11 +1301,11 @@
       </c>
       <c r="E17" s="3" cm="1">
         <f t="array" aca="1" ref="E17" ca="1">_xlfn.IFS(D17=1,'Ark1'!$C$2,D17=2, 'Ark1'!$C$3,D17=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F17" s="3" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">_xlfn.IFS(D17=1,'Ark1'!$D$2,D17=2, 'Ark1'!$D$3,D17=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1325,11 +1325,11 @@
       </c>
       <c r="E18" s="3" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">_xlfn.IFS(D18=1,'Ark1'!$C$2,D18=2, 'Ark1'!$C$3,D18=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F18" s="3" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">_xlfn.IFS(D18=1,'Ark1'!$D$2,D18=2, 'Ark1'!$D$3,D18=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,19 +1341,19 @@
       </c>
       <c r="C19" t="str" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">_xlfn.IFS(D19=1,"CPH",D19=2, "LON",D19=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="3" cm="1">
         <f t="array" aca="1" ref="E19" ca="1">_xlfn.IFS(D19=1,'Ark1'!$C$2,D19=2, 'Ark1'!$C$3,D19=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F19" s="3" cm="1">
         <f t="array" aca="1" ref="F19" ca="1">_xlfn.IFS(D19=1,'Ark1'!$D$2,D19=2, 'Ark1'!$D$3,D19=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1365,19 +1365,19 @@
       </c>
       <c r="C20" t="str" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">_xlfn.IFS(D20=1,"CPH",D20=2, "LON",D20=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="3" cm="1">
         <f t="array" aca="1" ref="E20" ca="1">_xlfn.IFS(D20=1,'Ark1'!$C$2,D20=2, 'Ark1'!$C$3,D20=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F20" s="3" cm="1">
         <f t="array" aca="1" ref="F20" ca="1">_xlfn.IFS(D20=1,'Ark1'!$D$2,D20=2, 'Ark1'!$D$3,D20=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,19 +1389,19 @@
       </c>
       <c r="C21" t="str" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">_xlfn.IFS(D21=1,"CPH",D21=2, "LON",D21=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E21" s="3" cm="1">
         <f t="array" aca="1" ref="E21" ca="1">_xlfn.IFS(D21=1,'Ark1'!$C$2,D21=2, 'Ark1'!$C$3,D21=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F21" s="3" cm="1">
         <f t="array" aca="1" ref="F21" ca="1">_xlfn.IFS(D21=1,'Ark1'!$D$2,D21=2, 'Ark1'!$D$3,D21=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1413,19 +1413,19 @@
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">_xlfn.IFS(D22=1,"CPH",D22=2, "LON",D22=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3" cm="1">
         <f t="array" aca="1" ref="E22" ca="1">_xlfn.IFS(D22=1,'Ark1'!$C$2,D22=2, 'Ark1'!$C$3,D22=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F22" s="3" cm="1">
         <f t="array" aca="1" ref="F22" ca="1">_xlfn.IFS(D22=1,'Ark1'!$D$2,D22=2, 'Ark1'!$D$3,D22=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1437,19 +1437,19 @@
       </c>
       <c r="C23" t="str" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">_xlfn.IFS(D23=1,"CPH",D23=2, "LON",D23=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E23" s="3" cm="1">
         <f t="array" aca="1" ref="E23" ca="1">_xlfn.IFS(D23=1,'Ark1'!$C$2,D23=2, 'Ark1'!$C$3,D23=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F23" s="3" cm="1">
         <f t="array" aca="1" ref="F23" ca="1">_xlfn.IFS(D23=1,'Ark1'!$D$2,D23=2, 'Ark1'!$D$3,D23=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1469,11 +1469,11 @@
       </c>
       <c r="E24" s="3" cm="1">
         <f t="array" aca="1" ref="E24" ca="1">_xlfn.IFS(D24=1,'Ark1'!$C$2,D24=2, 'Ark1'!$C$3,D24=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F24" s="3" cm="1">
         <f t="array" aca="1" ref="F24" ca="1">_xlfn.IFS(D24=1,'Ark1'!$D$2,D24=2, 'Ark1'!$D$3,D24=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,19 +1485,19 @@
       </c>
       <c r="C25" t="str" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">_xlfn.IFS(D25=1,"CPH",D25=2, "LON",D25=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="3" cm="1">
         <f t="array" aca="1" ref="E25" ca="1">_xlfn.IFS(D25=1,'Ark1'!$C$2,D25=2, 'Ark1'!$C$3,D25=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F25" s="3" cm="1">
         <f t="array" aca="1" ref="F25" ca="1">_xlfn.IFS(D25=1,'Ark1'!$D$2,D25=2, 'Ark1'!$D$3,D25=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1509,19 +1509,19 @@
       </c>
       <c r="C26" t="str" cm="1">
         <f t="array" aca="1" ref="C26" ca="1">_xlfn.IFS(D26=1,"CPH",D26=2, "LON",D26=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26" s="3" cm="1">
         <f t="array" aca="1" ref="E26" ca="1">_xlfn.IFS(D26=1,'Ark1'!$C$2,D26=2, 'Ark1'!$C$3,D26=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F26" s="3" cm="1">
         <f t="array" aca="1" ref="F26" ca="1">_xlfn.IFS(D26=1,'Ark1'!$D$2,D26=2, 'Ark1'!$D$3,D26=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1533,19 +1533,19 @@
       </c>
       <c r="C27" t="str" cm="1">
         <f t="array" aca="1" ref="C27" ca="1">_xlfn.IFS(D27=1,"CPH",D27=2, "LON",D27=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E27" s="3" cm="1">
         <f t="array" aca="1" ref="E27" ca="1">_xlfn.IFS(D27=1,'Ark1'!$C$2,D27=2, 'Ark1'!$C$3,D27=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F27" s="3" cm="1">
         <f t="array" aca="1" ref="F27" ca="1">_xlfn.IFS(D27=1,'Ark1'!$D$2,D27=2, 'Ark1'!$D$3,D27=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1565,11 +1565,11 @@
       </c>
       <c r="E28" s="3" cm="1">
         <f t="array" aca="1" ref="E28" ca="1">_xlfn.IFS(D28=1,'Ark1'!$C$2,D28=2, 'Ark1'!$C$3,D28=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F28" s="3" cm="1">
         <f t="array" aca="1" ref="F28" ca="1">_xlfn.IFS(D28=1,'Ark1'!$D$2,D28=2, 'Ark1'!$D$3,D28=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1589,11 +1589,11 @@
       </c>
       <c r="E29" s="3" cm="1">
         <f t="array" aca="1" ref="E29" ca="1">_xlfn.IFS(D29=1,'Ark1'!$C$2,D29=2, 'Ark1'!$C$3,D29=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F29" s="3" cm="1">
         <f t="array" aca="1" ref="F29" ca="1">_xlfn.IFS(D29=1,'Ark1'!$D$2,D29=2, 'Ark1'!$D$3,D29=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1605,19 +1605,19 @@
       </c>
       <c r="C30" t="str" cm="1">
         <f t="array" aca="1" ref="C30" ca="1">_xlfn.IFS(D30=1,"CPH",D30=2, "LON",D30=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="3" cm="1">
         <f t="array" aca="1" ref="E30" ca="1">_xlfn.IFS(D30=1,'Ark1'!$C$2,D30=2, 'Ark1'!$C$3,D30=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F30" s="3" cm="1">
         <f t="array" aca="1" ref="F30" ca="1">_xlfn.IFS(D30=1,'Ark1'!$D$2,D30=2, 'Ark1'!$D$3,D30=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1637,11 +1637,11 @@
       </c>
       <c r="E31" s="3" cm="1">
         <f t="array" aca="1" ref="E31" ca="1">_xlfn.IFS(D31=1,'Ark1'!$C$2,D31=2, 'Ark1'!$C$3,D31=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F31" s="3" cm="1">
         <f t="array" aca="1" ref="F31" ca="1">_xlfn.IFS(D31=1,'Ark1'!$D$2,D31=2, 'Ark1'!$D$3,D31=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1653,19 +1653,19 @@
       </c>
       <c r="C32" t="str" cm="1">
         <f t="array" aca="1" ref="C32" ca="1">_xlfn.IFS(D32=1,"CPH",D32=2, "LON",D32=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="3" cm="1">
         <f t="array" aca="1" ref="E32" ca="1">_xlfn.IFS(D32=1,'Ark1'!$C$2,D32=2, 'Ark1'!$C$3,D32=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F32" s="3" cm="1">
         <f t="array" aca="1" ref="F32" ca="1">_xlfn.IFS(D32=1,'Ark1'!$D$2,D32=2, 'Ark1'!$D$3,D32=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1677,19 +1677,19 @@
       </c>
       <c r="C33" t="str" cm="1">
         <f t="array" aca="1" ref="C33" ca="1">_xlfn.IFS(D33=1,"CPH",D33=2, "LON",D33=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E33" s="3" cm="1">
         <f t="array" aca="1" ref="E33" ca="1">_xlfn.IFS(D33=1,'Ark1'!$C$2,D33=2, 'Ark1'!$C$3,D33=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F33" s="3" cm="1">
         <f t="array" aca="1" ref="F33" ca="1">_xlfn.IFS(D33=1,'Ark1'!$D$2,D33=2, 'Ark1'!$D$3,D33=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1701,19 +1701,19 @@
       </c>
       <c r="C34" t="str" cm="1">
         <f t="array" aca="1" ref="C34" ca="1">_xlfn.IFS(D34=1,"CPH",D34=2, "LON",D34=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E34" s="3" cm="1">
         <f t="array" aca="1" ref="E34" ca="1">_xlfn.IFS(D34=1,'Ark1'!$C$2,D34=2, 'Ark1'!$C$3,D34=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F34" s="3" cm="1">
         <f t="array" aca="1" ref="F34" ca="1">_xlfn.IFS(D34=1,'Ark1'!$D$2,D34=2, 'Ark1'!$D$3,D34=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1733,11 +1733,11 @@
       </c>
       <c r="E35" s="3" cm="1">
         <f t="array" aca="1" ref="E35" ca="1">_xlfn.IFS(D35=1,'Ark1'!$C$2,D35=2, 'Ark1'!$C$3,D35=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F35" s="3" cm="1">
         <f t="array" aca="1" ref="F35" ca="1">_xlfn.IFS(D35=1,'Ark1'!$D$2,D35=2, 'Ark1'!$D$3,D35=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1749,19 +1749,19 @@
       </c>
       <c r="C36" t="str" cm="1">
         <f t="array" aca="1" ref="C36" ca="1">_xlfn.IFS(D36=1,"CPH",D36=2, "LON",D36=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="3" cm="1">
         <f t="array" aca="1" ref="E36" ca="1">_xlfn.IFS(D36=1,'Ark1'!$C$2,D36=2, 'Ark1'!$C$3,D36=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F36" s="3" cm="1">
         <f t="array" aca="1" ref="F36" ca="1">_xlfn.IFS(D36=1,'Ark1'!$D$2,D36=2, 'Ark1'!$D$3,D36=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1781,11 +1781,11 @@
       </c>
       <c r="E37" s="3" cm="1">
         <f t="array" aca="1" ref="E37" ca="1">_xlfn.IFS(D37=1,'Ark1'!$C$2,D37=2, 'Ark1'!$C$3,D37=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F37" s="3" cm="1">
         <f t="array" aca="1" ref="F37" ca="1">_xlfn.IFS(D37=1,'Ark1'!$D$2,D37=2, 'Ark1'!$D$3,D37=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1797,19 +1797,19 @@
       </c>
       <c r="C38" t="str" cm="1">
         <f t="array" aca="1" ref="C38" ca="1">_xlfn.IFS(D38=1,"CPH",D38=2, "LON",D38=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="3" cm="1">
         <f t="array" aca="1" ref="E38" ca="1">_xlfn.IFS(D38=1,'Ark1'!$C$2,D38=2, 'Ark1'!$C$3,D38=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F38" s="3" cm="1">
         <f t="array" aca="1" ref="F38" ca="1">_xlfn.IFS(D38=1,'Ark1'!$D$2,D38=2, 'Ark1'!$D$3,D38=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1821,19 +1821,19 @@
       </c>
       <c r="C39" t="str" cm="1">
         <f t="array" aca="1" ref="C39" ca="1">_xlfn.IFS(D39=1,"CPH",D39=2, "LON",D39=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="3" cm="1">
         <f t="array" aca="1" ref="E39" ca="1">_xlfn.IFS(D39=1,'Ark1'!$C$2,D39=2, 'Ark1'!$C$3,D39=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F39" s="3" cm="1">
         <f t="array" aca="1" ref="F39" ca="1">_xlfn.IFS(D39=1,'Ark1'!$D$2,D39=2, 'Ark1'!$D$3,D39=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1845,19 +1845,19 @@
       </c>
       <c r="C40" t="str" cm="1">
         <f t="array" aca="1" ref="C40" ca="1">_xlfn.IFS(D40=1,"CPH",D40=2, "LON",D40=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E40" s="3" cm="1">
         <f t="array" aca="1" ref="E40" ca="1">_xlfn.IFS(D40=1,'Ark1'!$C$2,D40=2, 'Ark1'!$C$3,D40=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F40" s="3" cm="1">
         <f t="array" aca="1" ref="F40" ca="1">_xlfn.IFS(D40=1,'Ark1'!$D$2,D40=2, 'Ark1'!$D$3,D40=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1869,19 +1869,19 @@
       </c>
       <c r="C41" t="str" cm="1">
         <f t="array" aca="1" ref="C41" ca="1">_xlfn.IFS(D41=1,"CPH",D41=2, "LON",D41=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="3" cm="1">
         <f t="array" aca="1" ref="E41" ca="1">_xlfn.IFS(D41=1,'Ark1'!$C$2,D41=2, 'Ark1'!$C$3,D41=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F41" s="3" cm="1">
         <f t="array" aca="1" ref="F41" ca="1">_xlfn.IFS(D41=1,'Ark1'!$D$2,D41=2, 'Ark1'!$D$3,D41=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1901,11 +1901,11 @@
       </c>
       <c r="E42" s="3" cm="1">
         <f t="array" aca="1" ref="E42" ca="1">_xlfn.IFS(D42=1,'Ark1'!$C$2,D42=2, 'Ark1'!$C$3,D42=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F42" s="3" cm="1">
         <f t="array" aca="1" ref="F42" ca="1">_xlfn.IFS(D42=1,'Ark1'!$D$2,D42=2, 'Ark1'!$D$3,D42=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,19 +1917,19 @@
       </c>
       <c r="C43" t="str" cm="1">
         <f t="array" aca="1" ref="C43" ca="1">_xlfn.IFS(D43=1,"CPH",D43=2, "LON",D43=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" s="3" cm="1">
         <f t="array" aca="1" ref="E43" ca="1">_xlfn.IFS(D43=1,'Ark1'!$C$2,D43=2, 'Ark1'!$C$3,D43=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F43" s="3" cm="1">
         <f t="array" aca="1" ref="F43" ca="1">_xlfn.IFS(D43=1,'Ark1'!$D$2,D43=2, 'Ark1'!$D$3,D43=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1941,19 +1941,19 @@
       </c>
       <c r="C44" t="str" cm="1">
         <f t="array" aca="1" ref="C44" ca="1">_xlfn.IFS(D44=1,"CPH",D44=2, "LON",D44=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E44" s="3" cm="1">
         <f t="array" aca="1" ref="E44" ca="1">_xlfn.IFS(D44=1,'Ark1'!$C$2,D44=2, 'Ark1'!$C$3,D44=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F44" s="3" cm="1">
         <f t="array" aca="1" ref="F44" ca="1">_xlfn.IFS(D44=1,'Ark1'!$D$2,D44=2, 'Ark1'!$D$3,D44=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,19 +1965,19 @@
       </c>
       <c r="C45" t="str" cm="1">
         <f t="array" aca="1" ref="C45" ca="1">_xlfn.IFS(D45=1,"CPH",D45=2, "LON",D45=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45" s="3" cm="1">
         <f t="array" aca="1" ref="E45" ca="1">_xlfn.IFS(D45=1,'Ark1'!$C$2,D45=2, 'Ark1'!$C$3,D45=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F45" s="3" cm="1">
         <f t="array" aca="1" ref="F45" ca="1">_xlfn.IFS(D45=1,'Ark1'!$D$2,D45=2, 'Ark1'!$D$3,D45=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1989,19 +1989,19 @@
       </c>
       <c r="C46" t="str" cm="1">
         <f t="array" aca="1" ref="C46" ca="1">_xlfn.IFS(D46=1,"CPH",D46=2, "LON",D46=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E46" s="3" cm="1">
         <f t="array" aca="1" ref="E46" ca="1">_xlfn.IFS(D46=1,'Ark1'!$C$2,D46=2, 'Ark1'!$C$3,D46=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F46" s="3" cm="1">
         <f t="array" aca="1" ref="F46" ca="1">_xlfn.IFS(D46=1,'Ark1'!$D$2,D46=2, 'Ark1'!$D$3,D46=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2021,11 +2021,11 @@
       </c>
       <c r="E47" s="3" cm="1">
         <f t="array" aca="1" ref="E47" ca="1">_xlfn.IFS(D47=1,'Ark1'!$C$2,D47=2, 'Ark1'!$C$3,D47=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F47" s="3" cm="1">
         <f t="array" aca="1" ref="F47" ca="1">_xlfn.IFS(D47=1,'Ark1'!$D$2,D47=2, 'Ark1'!$D$3,D47=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2045,11 +2045,11 @@
       </c>
       <c r="E48" s="3" cm="1">
         <f t="array" aca="1" ref="E48" ca="1">_xlfn.IFS(D48=1,'Ark1'!$C$2,D48=2, 'Ark1'!$C$3,D48=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F48" s="3" cm="1">
         <f t="array" aca="1" ref="F48" ca="1">_xlfn.IFS(D48=1,'Ark1'!$D$2,D48=2, 'Ark1'!$D$3,D48=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2069,11 +2069,11 @@
       </c>
       <c r="E49" s="3" cm="1">
         <f t="array" aca="1" ref="E49" ca="1">_xlfn.IFS(D49=1,'Ark1'!$C$2,D49=2, 'Ark1'!$C$3,D49=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F49" s="3" cm="1">
         <f t="array" aca="1" ref="F49" ca="1">_xlfn.IFS(D49=1,'Ark1'!$D$2,D49=2, 'Ark1'!$D$3,D49=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2093,11 +2093,11 @@
       </c>
       <c r="E50" s="3" cm="1">
         <f t="array" aca="1" ref="E50" ca="1">_xlfn.IFS(D50=1,'Ark1'!$C$2,D50=2, 'Ark1'!$C$3,D50=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F50" s="3" cm="1">
         <f t="array" aca="1" ref="F50" ca="1">_xlfn.IFS(D50=1,'Ark1'!$D$2,D50=2, 'Ark1'!$D$3,D50=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2117,11 +2117,11 @@
       </c>
       <c r="E51" s="3" cm="1">
         <f t="array" aca="1" ref="E51" ca="1">_xlfn.IFS(D51=1,'Ark1'!$C$2,D51=2, 'Ark1'!$C$3,D51=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F51" s="3" cm="1">
         <f t="array" aca="1" ref="F51" ca="1">_xlfn.IFS(D51=1,'Ark1'!$D$2,D51=2, 'Ark1'!$D$3,D51=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="E52" s="3" cm="1">
         <f t="array" aca="1" ref="E52" ca="1">_xlfn.IFS(D52=1,'Ark1'!$C$2,D52=2, 'Ark1'!$C$3,D52=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F52" s="3" cm="1">
         <f t="array" aca="1" ref="F52" ca="1">_xlfn.IFS(D52=1,'Ark1'!$D$2,D52=2, 'Ark1'!$D$3,D52=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2165,11 +2165,11 @@
       </c>
       <c r="E53" s="3" cm="1">
         <f t="array" aca="1" ref="E53" ca="1">_xlfn.IFS(D53=1,'Ark1'!$C$2,D53=2, 'Ark1'!$C$3,D53=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F53" s="3" cm="1">
         <f t="array" aca="1" ref="F53" ca="1">_xlfn.IFS(D53=1,'Ark1'!$D$2,D53=2, 'Ark1'!$D$3,D53=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2181,19 +2181,19 @@
       </c>
       <c r="C54" t="str" cm="1">
         <f t="array" aca="1" ref="C54" ca="1">_xlfn.IFS(D54=1,"CPH",D54=2, "LON",D54=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E54" s="3" cm="1">
         <f t="array" aca="1" ref="E54" ca="1">_xlfn.IFS(D54=1,'Ark1'!$C$2,D54=2, 'Ark1'!$C$3,D54=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F54" s="3" cm="1">
         <f t="array" aca="1" ref="F54" ca="1">_xlfn.IFS(D54=1,'Ark1'!$D$2,D54=2, 'Ark1'!$D$3,D54=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="E55" s="3" cm="1">
         <f t="array" aca="1" ref="E55" ca="1">_xlfn.IFS(D55=1,'Ark1'!$C$2,D55=2, 'Ark1'!$C$3,D55=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F55" s="3" cm="1">
         <f t="array" aca="1" ref="F55" ca="1">_xlfn.IFS(D55=1,'Ark1'!$D$2,D55=2, 'Ark1'!$D$3,D55=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,19 +2229,19 @@
       </c>
       <c r="C56" t="str" cm="1">
         <f t="array" aca="1" ref="C56" ca="1">_xlfn.IFS(D56=1,"CPH",D56=2, "LON",D56=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E56" s="3" cm="1">
         <f t="array" aca="1" ref="E56" ca="1">_xlfn.IFS(D56=1,'Ark1'!$C$2,D56=2, 'Ark1'!$C$3,D56=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F56" s="3" cm="1">
         <f t="array" aca="1" ref="F56" ca="1">_xlfn.IFS(D56=1,'Ark1'!$D$2,D56=2, 'Ark1'!$D$3,D56=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2253,19 +2253,19 @@
       </c>
       <c r="C57" t="str" cm="1">
         <f t="array" aca="1" ref="C57" ca="1">_xlfn.IFS(D57=1,"CPH",D57=2, "LON",D57=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" s="3" cm="1">
         <f t="array" aca="1" ref="E57" ca="1">_xlfn.IFS(D57=1,'Ark1'!$C$2,D57=2, 'Ark1'!$C$3,D57=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F57" s="3" cm="1">
         <f t="array" aca="1" ref="F57" ca="1">_xlfn.IFS(D57=1,'Ark1'!$D$2,D57=2, 'Ark1'!$D$3,D57=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2277,19 +2277,19 @@
       </c>
       <c r="C58" t="str" cm="1">
         <f t="array" aca="1" ref="C58" ca="1">_xlfn.IFS(D58=1,"CPH",D58=2, "LON",D58=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E58" s="3" cm="1">
         <f t="array" aca="1" ref="E58" ca="1">_xlfn.IFS(D58=1,'Ark1'!$C$2,D58=2, 'Ark1'!$C$3,D58=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F58" s="3" cm="1">
         <f t="array" aca="1" ref="F58" ca="1">_xlfn.IFS(D58=1,'Ark1'!$D$2,D58=2, 'Ark1'!$D$3,D58=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2301,19 +2301,19 @@
       </c>
       <c r="C59" t="str" cm="1">
         <f t="array" aca="1" ref="C59" ca="1">_xlfn.IFS(D59=1,"CPH",D59=2, "LON",D59=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E59" s="3" cm="1">
         <f t="array" aca="1" ref="E59" ca="1">_xlfn.IFS(D59=1,'Ark1'!$C$2,D59=2, 'Ark1'!$C$3,D59=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F59" s="3" cm="1">
         <f t="array" aca="1" ref="F59" ca="1">_xlfn.IFS(D59=1,'Ark1'!$D$2,D59=2, 'Ark1'!$D$3,D59=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2325,19 +2325,19 @@
       </c>
       <c r="C60" t="str" cm="1">
         <f t="array" aca="1" ref="C60" ca="1">_xlfn.IFS(D60=1,"CPH",D60=2, "LON",D60=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E60" s="3" cm="1">
         <f t="array" aca="1" ref="E60" ca="1">_xlfn.IFS(D60=1,'Ark1'!$C$2,D60=2, 'Ark1'!$C$3,D60=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F60" s="3" cm="1">
         <f t="array" aca="1" ref="F60" ca="1">_xlfn.IFS(D60=1,'Ark1'!$D$2,D60=2, 'Ark1'!$D$3,D60=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2357,11 +2357,11 @@
       </c>
       <c r="E61" s="3" cm="1">
         <f t="array" aca="1" ref="E61" ca="1">_xlfn.IFS(D61=1,'Ark1'!$C$2,D61=2, 'Ark1'!$C$3,D61=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F61" s="3" cm="1">
         <f t="array" aca="1" ref="F61" ca="1">_xlfn.IFS(D61=1,'Ark1'!$D$2,D61=2, 'Ark1'!$D$3,D61=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2373,19 +2373,19 @@
       </c>
       <c r="C62" t="str" cm="1">
         <f t="array" aca="1" ref="C62" ca="1">_xlfn.IFS(D62=1,"CPH",D62=2, "LON",D62=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62" s="3" cm="1">
         <f t="array" aca="1" ref="E62" ca="1">_xlfn.IFS(D62=1,'Ark1'!$C$2,D62=2, 'Ark1'!$C$3,D62=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F62" s="3" cm="1">
         <f t="array" aca="1" ref="F62" ca="1">_xlfn.IFS(D62=1,'Ark1'!$D$2,D62=2, 'Ark1'!$D$3,D62=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2397,19 +2397,19 @@
       </c>
       <c r="C63" t="str" cm="1">
         <f t="array" aca="1" ref="C63" ca="1">_xlfn.IFS(D63=1,"CPH",D63=2, "LON",D63=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E63" s="3" cm="1">
         <f t="array" aca="1" ref="E63" ca="1">_xlfn.IFS(D63=1,'Ark1'!$C$2,D63=2, 'Ark1'!$C$3,D63=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F63" s="3" cm="1">
         <f t="array" aca="1" ref="F63" ca="1">_xlfn.IFS(D63=1,'Ark1'!$D$2,D63=2, 'Ark1'!$D$3,D63=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2429,11 +2429,11 @@
       </c>
       <c r="E64" s="3" cm="1">
         <f t="array" aca="1" ref="E64" ca="1">_xlfn.IFS(D64=1,'Ark1'!$C$2,D64=2, 'Ark1'!$C$3,D64=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F64" s="3" cm="1">
         <f t="array" aca="1" ref="F64" ca="1">_xlfn.IFS(D64=1,'Ark1'!$D$2,D64=2, 'Ark1'!$D$3,D64=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2445,19 +2445,19 @@
       </c>
       <c r="C65" t="str" cm="1">
         <f t="array" aca="1" ref="C65" ca="1">_xlfn.IFS(D65=1,"CPH",D65=2, "LON",D65=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65" s="3" cm="1">
         <f t="array" aca="1" ref="E65" ca="1">_xlfn.IFS(D65=1,'Ark1'!$C$2,D65=2, 'Ark1'!$C$3,D65=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F65" s="3" cm="1">
         <f t="array" aca="1" ref="F65" ca="1">_xlfn.IFS(D65=1,'Ark1'!$D$2,D65=2, 'Ark1'!$D$3,D65=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,19 +2469,19 @@
       </c>
       <c r="C66" t="str" cm="1">
         <f t="array" aca="1" ref="C66" ca="1">_xlfn.IFS(D66=1,"CPH",D66=2, "LON",D66=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E66" s="3" cm="1">
         <f t="array" aca="1" ref="E66" ca="1">_xlfn.IFS(D66=1,'Ark1'!$C$2,D66=2, 'Ark1'!$C$3,D66=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F66" s="3" cm="1">
         <f t="array" aca="1" ref="F66" ca="1">_xlfn.IFS(D66=1,'Ark1'!$D$2,D66=2, 'Ark1'!$D$3,D66=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2493,19 +2493,19 @@
       </c>
       <c r="C67" t="str" cm="1">
         <f t="array" aca="1" ref="C67" ca="1">_xlfn.IFS(D67=1,"CPH",D67=2, "LON",D67=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D67">
         <f t="shared" ref="D67:D101" ca="1" si="1">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E67" s="3" cm="1">
         <f t="array" aca="1" ref="E67" ca="1">_xlfn.IFS(D67=1,'Ark1'!$C$2,D67=2, 'Ark1'!$C$3,D67=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F67" s="3" cm="1">
         <f t="array" aca="1" ref="F67" ca="1">_xlfn.IFS(D67=1,'Ark1'!$D$2,D67=2, 'Ark1'!$D$3,D67=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2517,19 +2517,19 @@
       </c>
       <c r="C68" t="str" cm="1">
         <f t="array" aca="1" ref="C68" ca="1">_xlfn.IFS(D68=1,"CPH",D68=2, "LON",D68=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E68" s="3" cm="1">
         <f t="array" aca="1" ref="E68" ca="1">_xlfn.IFS(D68=1,'Ark1'!$C$2,D68=2, 'Ark1'!$C$3,D68=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F68" s="3" cm="1">
         <f t="array" aca="1" ref="F68" ca="1">_xlfn.IFS(D68=1,'Ark1'!$D$2,D68=2, 'Ark1'!$D$3,D68=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2541,19 +2541,19 @@
       </c>
       <c r="C69" t="str" cm="1">
         <f t="array" aca="1" ref="C69" ca="1">_xlfn.IFS(D69=1,"CPH",D69=2, "LON",D69=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E69" s="3" cm="1">
         <f t="array" aca="1" ref="E69" ca="1">_xlfn.IFS(D69=1,'Ark1'!$C$2,D69=2, 'Ark1'!$C$3,D69=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F69" s="3" cm="1">
         <f t="array" aca="1" ref="F69" ca="1">_xlfn.IFS(D69=1,'Ark1'!$D$2,D69=2, 'Ark1'!$D$3,D69=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2573,11 +2573,11 @@
       </c>
       <c r="E70" s="3" cm="1">
         <f t="array" aca="1" ref="E70" ca="1">_xlfn.IFS(D70=1,'Ark1'!$C$2,D70=2, 'Ark1'!$C$3,D70=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F70" s="3" cm="1">
         <f t="array" aca="1" ref="F70" ca="1">_xlfn.IFS(D70=1,'Ark1'!$D$2,D70=2, 'Ark1'!$D$3,D70=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2589,19 +2589,19 @@
       </c>
       <c r="C71" t="str" cm="1">
         <f t="array" aca="1" ref="C71" ca="1">_xlfn.IFS(D71=1,"CPH",D71=2, "LON",D71=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E71" s="3" cm="1">
         <f t="array" aca="1" ref="E71" ca="1">_xlfn.IFS(D71=1,'Ark1'!$C$2,D71=2, 'Ark1'!$C$3,D71=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F71" s="3" cm="1">
         <f t="array" aca="1" ref="F71" ca="1">_xlfn.IFS(D71=1,'Ark1'!$D$2,D71=2, 'Ark1'!$D$3,D71=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2613,19 +2613,19 @@
       </c>
       <c r="C72" t="str" cm="1">
         <f t="array" aca="1" ref="C72" ca="1">_xlfn.IFS(D72=1,"CPH",D72=2, "LON",D72=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E72" s="3" cm="1">
         <f t="array" aca="1" ref="E72" ca="1">_xlfn.IFS(D72=1,'Ark1'!$C$2,D72=2, 'Ark1'!$C$3,D72=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F72" s="3" cm="1">
         <f t="array" aca="1" ref="F72" ca="1">_xlfn.IFS(D72=1,'Ark1'!$D$2,D72=2, 'Ark1'!$D$3,D72=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2645,11 +2645,11 @@
       </c>
       <c r="E73" s="3" cm="1">
         <f t="array" aca="1" ref="E73" ca="1">_xlfn.IFS(D73=1,'Ark1'!$C$2,D73=2, 'Ark1'!$C$3,D73=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F73" s="3" cm="1">
         <f t="array" aca="1" ref="F73" ca="1">_xlfn.IFS(D73=1,'Ark1'!$D$2,D73=2, 'Ark1'!$D$3,D73=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2669,11 +2669,11 @@
       </c>
       <c r="E74" s="3" cm="1">
         <f t="array" aca="1" ref="E74" ca="1">_xlfn.IFS(D74=1,'Ark1'!$C$2,D74=2, 'Ark1'!$C$3,D74=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F74" s="3" cm="1">
         <f t="array" aca="1" ref="F74" ca="1">_xlfn.IFS(D74=1,'Ark1'!$D$2,D74=2, 'Ark1'!$D$3,D74=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2685,19 +2685,19 @@
       </c>
       <c r="C75" t="str" cm="1">
         <f t="array" aca="1" ref="C75" ca="1">_xlfn.IFS(D75=1,"CPH",D75=2, "LON",D75=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E75" s="3" cm="1">
         <f t="array" aca="1" ref="E75" ca="1">_xlfn.IFS(D75=1,'Ark1'!$C$2,D75=2, 'Ark1'!$C$3,D75=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F75" s="3" cm="1">
         <f t="array" aca="1" ref="F75" ca="1">_xlfn.IFS(D75=1,'Ark1'!$D$2,D75=2, 'Ark1'!$D$3,D75=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2717,11 +2717,11 @@
       </c>
       <c r="E76" s="3" cm="1">
         <f t="array" aca="1" ref="E76" ca="1">_xlfn.IFS(D76=1,'Ark1'!$C$2,D76=2, 'Ark1'!$C$3,D76=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F76" s="3" cm="1">
         <f t="array" aca="1" ref="F76" ca="1">_xlfn.IFS(D76=1,'Ark1'!$D$2,D76=2, 'Ark1'!$D$3,D76=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2741,11 +2741,11 @@
       </c>
       <c r="E77" s="3" cm="1">
         <f t="array" aca="1" ref="E77" ca="1">_xlfn.IFS(D77=1,'Ark1'!$C$2,D77=2, 'Ark1'!$C$3,D77=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F77" s="3" cm="1">
         <f t="array" aca="1" ref="F77" ca="1">_xlfn.IFS(D77=1,'Ark1'!$D$2,D77=2, 'Ark1'!$D$3,D77=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2757,19 +2757,19 @@
       </c>
       <c r="C78" t="str" cm="1">
         <f t="array" aca="1" ref="C78" ca="1">_xlfn.IFS(D78=1,"CPH",D78=2, "LON",D78=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E78" s="3" cm="1">
         <f t="array" aca="1" ref="E78" ca="1">_xlfn.IFS(D78=1,'Ark1'!$C$2,D78=2, 'Ark1'!$C$3,D78=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F78" s="3" cm="1">
         <f t="array" aca="1" ref="F78" ca="1">_xlfn.IFS(D78=1,'Ark1'!$D$2,D78=2, 'Ark1'!$D$3,D78=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2789,11 +2789,11 @@
       </c>
       <c r="E79" s="3" cm="1">
         <f t="array" aca="1" ref="E79" ca="1">_xlfn.IFS(D79=1,'Ark1'!$C$2,D79=2, 'Ark1'!$C$3,D79=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F79" s="3" cm="1">
         <f t="array" aca="1" ref="F79" ca="1">_xlfn.IFS(D79=1,'Ark1'!$D$2,D79=2, 'Ark1'!$D$3,D79=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2805,19 +2805,19 @@
       </c>
       <c r="C80" t="str" cm="1">
         <f t="array" aca="1" ref="C80" ca="1">_xlfn.IFS(D80=1,"CPH",D80=2, "LON",D80=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E80" s="3" cm="1">
         <f t="array" aca="1" ref="E80" ca="1">_xlfn.IFS(D80=1,'Ark1'!$C$2,D80=2, 'Ark1'!$C$3,D80=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F80" s="3" cm="1">
         <f t="array" aca="1" ref="F80" ca="1">_xlfn.IFS(D80=1,'Ark1'!$D$2,D80=2, 'Ark1'!$D$3,D80=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2837,11 +2837,11 @@
       </c>
       <c r="E81" s="3" cm="1">
         <f t="array" aca="1" ref="E81" ca="1">_xlfn.IFS(D81=1,'Ark1'!$C$2,D81=2, 'Ark1'!$C$3,D81=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F81" s="3" cm="1">
         <f t="array" aca="1" ref="F81" ca="1">_xlfn.IFS(D81=1,'Ark1'!$D$2,D81=2, 'Ark1'!$D$3,D81=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2853,19 +2853,19 @@
       </c>
       <c r="C82" t="str" cm="1">
         <f t="array" aca="1" ref="C82" ca="1">_xlfn.IFS(D82=1,"CPH",D82=2, "LON",D82=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E82" s="3" cm="1">
         <f t="array" aca="1" ref="E82" ca="1">_xlfn.IFS(D82=1,'Ark1'!$C$2,D82=2, 'Ark1'!$C$3,D82=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F82" s="3" cm="1">
         <f t="array" aca="1" ref="F82" ca="1">_xlfn.IFS(D82=1,'Ark1'!$D$2,D82=2, 'Ark1'!$D$3,D82=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2885,11 +2885,11 @@
       </c>
       <c r="E83" s="3" cm="1">
         <f t="array" aca="1" ref="E83" ca="1">_xlfn.IFS(D83=1,'Ark1'!$C$2,D83=2, 'Ark1'!$C$3,D83=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F83" s="3" cm="1">
         <f t="array" aca="1" ref="F83" ca="1">_xlfn.IFS(D83=1,'Ark1'!$D$2,D83=2, 'Ark1'!$D$3,D83=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2909,11 +2909,11 @@
       </c>
       <c r="E84" s="3" cm="1">
         <f t="array" aca="1" ref="E84" ca="1">_xlfn.IFS(D84=1,'Ark1'!$C$2,D84=2, 'Ark1'!$C$3,D84=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F84" s="3" cm="1">
         <f t="array" aca="1" ref="F84" ca="1">_xlfn.IFS(D84=1,'Ark1'!$D$2,D84=2, 'Ark1'!$D$3,D84=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2925,19 +2925,19 @@
       </c>
       <c r="C85" t="str" cm="1">
         <f t="array" aca="1" ref="C85" ca="1">_xlfn.IFS(D85=1,"CPH",D85=2, "LON",D85=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E85" s="3" cm="1">
         <f t="array" aca="1" ref="E85" ca="1">_xlfn.IFS(D85=1,'Ark1'!$C$2,D85=2, 'Ark1'!$C$3,D85=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F85" s="3" cm="1">
         <f t="array" aca="1" ref="F85" ca="1">_xlfn.IFS(D85=1,'Ark1'!$D$2,D85=2, 'Ark1'!$D$3,D85=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2949,19 +2949,19 @@
       </c>
       <c r="C86" t="str" cm="1">
         <f t="array" aca="1" ref="C86" ca="1">_xlfn.IFS(D86=1,"CPH",D86=2, "LON",D86=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E86" s="3" cm="1">
         <f t="array" aca="1" ref="E86" ca="1">_xlfn.IFS(D86=1,'Ark1'!$C$2,D86=2, 'Ark1'!$C$3,D86=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F86" s="3" cm="1">
         <f t="array" aca="1" ref="F86" ca="1">_xlfn.IFS(D86=1,'Ark1'!$D$2,D86=2, 'Ark1'!$D$3,D86=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2973,19 +2973,19 @@
       </c>
       <c r="C87" t="str" cm="1">
         <f t="array" aca="1" ref="C87" ca="1">_xlfn.IFS(D87=1,"CPH",D87=2, "LON",D87=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E87" s="3" cm="1">
         <f t="array" aca="1" ref="E87" ca="1">_xlfn.IFS(D87=1,'Ark1'!$C$2,D87=2, 'Ark1'!$C$3,D87=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F87" s="3" cm="1">
         <f t="array" aca="1" ref="F87" ca="1">_xlfn.IFS(D87=1,'Ark1'!$D$2,D87=2, 'Ark1'!$D$3,D87=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2997,19 +2997,19 @@
       </c>
       <c r="C88" t="str" cm="1">
         <f t="array" aca="1" ref="C88" ca="1">_xlfn.IFS(D88=1,"CPH",D88=2, "LON",D88=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E88" s="3" cm="1">
         <f t="array" aca="1" ref="E88" ca="1">_xlfn.IFS(D88=1,'Ark1'!$C$2,D88=2, 'Ark1'!$C$3,D88=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F88" s="3" cm="1">
         <f t="array" aca="1" ref="F88" ca="1">_xlfn.IFS(D88=1,'Ark1'!$D$2,D88=2, 'Ark1'!$D$3,D88=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3021,19 +3021,19 @@
       </c>
       <c r="C89" t="str" cm="1">
         <f t="array" aca="1" ref="C89" ca="1">_xlfn.IFS(D89=1,"CPH",D89=2, "LON",D89=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E89" s="3" cm="1">
         <f t="array" aca="1" ref="E89" ca="1">_xlfn.IFS(D89=1,'Ark1'!$C$2,D89=2, 'Ark1'!$C$3,D89=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F89" s="3" cm="1">
         <f t="array" aca="1" ref="F89" ca="1">_xlfn.IFS(D89=1,'Ark1'!$D$2,D89=2, 'Ark1'!$D$3,D89=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3045,19 +3045,19 @@
       </c>
       <c r="C90" t="str" cm="1">
         <f t="array" aca="1" ref="C90" ca="1">_xlfn.IFS(D90=1,"CPH",D90=2, "LON",D90=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E90" s="3" cm="1">
         <f t="array" aca="1" ref="E90" ca="1">_xlfn.IFS(D90=1,'Ark1'!$C$2,D90=2, 'Ark1'!$C$3,D90=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F90" s="3" cm="1">
         <f t="array" aca="1" ref="F90" ca="1">_xlfn.IFS(D90=1,'Ark1'!$D$2,D90=2, 'Ark1'!$D$3,D90=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3069,19 +3069,19 @@
       </c>
       <c r="C91" t="str" cm="1">
         <f t="array" aca="1" ref="C91" ca="1">_xlfn.IFS(D91=1,"CPH",D91=2, "LON",D91=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E91" s="3" cm="1">
         <f t="array" aca="1" ref="E91" ca="1">_xlfn.IFS(D91=1,'Ark1'!$C$2,D91=2, 'Ark1'!$C$3,D91=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F91" s="3" cm="1">
         <f t="array" aca="1" ref="F91" ca="1">_xlfn.IFS(D91=1,'Ark1'!$D$2,D91=2, 'Ark1'!$D$3,D91=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3093,19 +3093,19 @@
       </c>
       <c r="C92" t="str" cm="1">
         <f t="array" aca="1" ref="C92" ca="1">_xlfn.IFS(D92=1,"CPH",D92=2, "LON",D92=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E92" s="3" cm="1">
         <f t="array" aca="1" ref="E92" ca="1">_xlfn.IFS(D92=1,'Ark1'!$C$2,D92=2, 'Ark1'!$C$3,D92=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F92" s="3" cm="1">
         <f t="array" aca="1" ref="F92" ca="1">_xlfn.IFS(D92=1,'Ark1'!$D$2,D92=2, 'Ark1'!$D$3,D92=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3125,11 +3125,11 @@
       </c>
       <c r="E93" s="3" cm="1">
         <f t="array" aca="1" ref="E93" ca="1">_xlfn.IFS(D93=1,'Ark1'!$C$2,D93=2, 'Ark1'!$C$3,D93=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F93" s="3" cm="1">
         <f t="array" aca="1" ref="F93" ca="1">_xlfn.IFS(D93=1,'Ark1'!$D$2,D93=2, 'Ark1'!$D$3,D93=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3141,19 +3141,19 @@
       </c>
       <c r="C94" t="str" cm="1">
         <f t="array" aca="1" ref="C94" ca="1">_xlfn.IFS(D94=1,"CPH",D94=2, "LON",D94=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D94">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E94" s="3" cm="1">
         <f t="array" aca="1" ref="E94" ca="1">_xlfn.IFS(D94=1,'Ark1'!$C$2,D94=2, 'Ark1'!$C$3,D94=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F94" s="3" cm="1">
         <f t="array" aca="1" ref="F94" ca="1">_xlfn.IFS(D94=1,'Ark1'!$D$2,D94=2, 'Ark1'!$D$3,D94=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3165,19 +3165,19 @@
       </c>
       <c r="C95" t="str" cm="1">
         <f t="array" aca="1" ref="C95" ca="1">_xlfn.IFS(D95=1,"CPH",D95=2, "LON",D95=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E95" s="3" cm="1">
         <f t="array" aca="1" ref="E95" ca="1">_xlfn.IFS(D95=1,'Ark1'!$C$2,D95=2, 'Ark1'!$C$3,D95=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F95" s="3" cm="1">
         <f t="array" aca="1" ref="F95" ca="1">_xlfn.IFS(D95=1,'Ark1'!$D$2,D95=2, 'Ark1'!$D$3,D95=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3189,19 +3189,19 @@
       </c>
       <c r="C96" t="str" cm="1">
         <f t="array" aca="1" ref="C96" ca="1">_xlfn.IFS(D96=1,"CPH",D96=2, "LON",D96=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D96">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E96" s="3" cm="1">
         <f t="array" aca="1" ref="E96" ca="1">_xlfn.IFS(D96=1,'Ark1'!$C$2,D96=2, 'Ark1'!$C$3,D96=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F96" s="3" cm="1">
         <f t="array" aca="1" ref="F96" ca="1">_xlfn.IFS(D96=1,'Ark1'!$D$2,D96=2, 'Ark1'!$D$3,D96=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3213,19 +3213,19 @@
       </c>
       <c r="C97" t="str" cm="1">
         <f t="array" aca="1" ref="C97" ca="1">_xlfn.IFS(D97=1,"CPH",D97=2, "LON",D97=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D97">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E97" s="3" cm="1">
         <f t="array" aca="1" ref="E97" ca="1">_xlfn.IFS(D97=1,'Ark1'!$C$2,D97=2, 'Ark1'!$C$3,D97=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F97" s="3" cm="1">
         <f t="array" aca="1" ref="F97" ca="1">_xlfn.IFS(D97=1,'Ark1'!$D$2,D97=2, 'Ark1'!$D$3,D97=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3237,19 +3237,19 @@
       </c>
       <c r="C98" t="str" cm="1">
         <f t="array" aca="1" ref="C98" ca="1">_xlfn.IFS(D98=1,"CPH",D98=2, "LON",D98=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E98" s="3" cm="1">
         <f t="array" aca="1" ref="E98" ca="1">_xlfn.IFS(D98=1,'Ark1'!$C$2,D98=2, 'Ark1'!$C$3,D98=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F98" s="3" cm="1">
         <f t="array" aca="1" ref="F98" ca="1">_xlfn.IFS(D98=1,'Ark1'!$D$2,D98=2, 'Ark1'!$D$3,D98=3,'Ark1'!$D$4)</f>
-        <v>44260.626889120365</v>
+        <v>44263.759250347219</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3261,19 +3261,19 @@
       </c>
       <c r="C99" t="str" cm="1">
         <f t="array" aca="1" ref="C99" ca="1">_xlfn.IFS(D99=1,"CPH",D99=2, "LON",D99=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E99" s="3" cm="1">
         <f t="array" aca="1" ref="E99" ca="1">_xlfn.IFS(D99=1,'Ark1'!$C$2,D99=2, 'Ark1'!$C$3,D99=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F99" s="3" cm="1">
         <f t="array" aca="1" ref="F99" ca="1">_xlfn.IFS(D99=1,'Ark1'!$D$2,D99=2, 'Ark1'!$D$3,D99=3,'Ark1'!$D$4)</f>
-        <v>44260.626194675926</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3285,19 +3285,19 @@
       </c>
       <c r="C100" t="str" cm="1">
         <f t="array" aca="1" ref="C100" ca="1">_xlfn.IFS(D100=1,"CPH",D100=2, "LON",D100=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E100" s="3" cm="1">
         <f t="array" aca="1" ref="E100" ca="1">_xlfn.IFS(D100=1,'Ark1'!$C$2,D100=2, 'Ark1'!$C$3,D100=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F100" s="3" cm="1">
         <f t="array" aca="1" ref="F100" ca="1">_xlfn.IFS(D100=1,'Ark1'!$D$2,D100=2, 'Ark1'!$D$3,D100=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.759944791665</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3309,19 +3309,19 @@
       </c>
       <c r="C101" t="str" cm="1">
         <f t="array" aca="1" ref="C101" ca="1">_xlfn.IFS(D101=1,"CPH",D101=2, "LON",D101=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E101" s="3" cm="1">
         <f t="array" aca="1" ref="E101" ca="1">_xlfn.IFS(D101=1,'Ark1'!$C$2,D101=2, 'Ark1'!$C$3,D101=3,'Ark1'!$C$4)</f>
-        <v>44260.623416898146</v>
+        <v>44263.757167013886</v>
       </c>
       <c r="F101" s="3" cm="1">
         <f t="array" aca="1" ref="F101" ca="1">_xlfn.IFS(D101=1,'Ark1'!$D$2,D101=2, 'Ark1'!$D$3,D101=3,'Ark1'!$D$4)</f>
-        <v>44260.625500231479</v>
+        <v>44263.760639236105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small changes on console BaggageHandlingSystem
</commit_message>
<xml_diff>
--- a/ThreadSync/ThreadSync_BaggageHandlingSystem/BaggageHandlingSystem/bin/Debug/ReservationGenerator.xlsx
+++ b/ThreadSync/ThreadSync_BaggageHandlingSystem/BaggageHandlingSystem/bin/Debug/ReservationGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjedt\source\repos_git\_SchoolWork\ThreadSync\ThreadSync_BaggageHandlingSystem\BaggageHandlingSystem\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11A1A59-0912-48AC-91DA-BB9CFACB6B2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C462518-AF6E-4C88-86A2-0F9F80899BB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9C29B736-50C8-4AEB-AA05-EAA881D5DAC3}"/>
+    <workbookView xWindow="11430" yWindow="4575" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{9C29B736-50C8-4AEB-AA05-EAA881D5DAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -785,11 +785,11 @@
       </c>
       <c r="C2" s="1">
         <f ca="1">NOW()+2/24/60</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">C2+3/24/60</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -801,11 +801,11 @@
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C4" ca="1" si="0">NOW()+2/24/60</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="D3" s="1">
         <f ca="1">C3+5/24/60</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,11 +817,11 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="D4" s="1">
         <f ca="1">C4+4/24/60</f>
-        <v>44263.759944791665</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -833,11 +833,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">D2+2/24/60</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
       <c r="D5" s="1">
         <f ca="1">C5+4/24/60</f>
-        <v>44263.763417013884</v>
+        <v>44264.395901041666</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -849,11 +849,11 @@
       </c>
       <c r="C6" s="1">
         <f ca="1">D3+1/24/60</f>
-        <v>44263.761333680552</v>
+        <v>44264.393817708333</v>
       </c>
       <c r="D6" s="1">
         <f ca="1">C6+3/24/60</f>
-        <v>44263.763417013884</v>
+        <v>44264.395901041666</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -865,11 +865,11 @@
       </c>
       <c r="C7" s="1">
         <f ca="1">D4+2/24/60</f>
-        <v>44263.761333680552</v>
+        <v>44264.393817708333</v>
       </c>
       <c r="D7" s="1">
         <f ca="1">C7+5/24/60</f>
-        <v>44263.764805902771</v>
+        <v>44264.397289930552</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F013B4FB-C891-40D9-903B-3DAA8FC8D684}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F101"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,19 +933,19 @@
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">_xlfn.IFS(D2=1,"CPH",D2=2, "LON",D2=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="3" cm="1">
         <f t="array" aca="1" ref="E2" ca="1">_xlfn.IFS(D2=1,'Ark1'!$C$2,D2=2, 'Ark1'!$C$3,D2=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F2" s="3" cm="1">
         <f t="array" aca="1" ref="F2" ca="1">_xlfn.IFS(D2=1,'Ark1'!$D$2,D2=2, 'Ark1'!$D$3,D2=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -965,11 +965,11 @@
       </c>
       <c r="E3" s="3" cm="1">
         <f t="array" aca="1" ref="E3" ca="1">_xlfn.IFS(D3=1,'Ark1'!$C$2,D3=2, 'Ark1'!$C$3,D3=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F3" s="3" cm="1">
         <f t="array" aca="1" ref="F3" ca="1">_xlfn.IFS(D3=1,'Ark1'!$D$2,D3=2, 'Ark1'!$D$3,D3=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -981,19 +981,19 @@
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">_xlfn.IFS(D4=1,"CPH",D4=2, "LON",D4=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D66" ca="1" si="0">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" cm="1">
         <f t="array" aca="1" ref="E4" ca="1">_xlfn.IFS(D4=1,'Ark1'!$C$2,D4=2, 'Ark1'!$C$3,D4=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F4" s="3" cm="1">
         <f t="array" aca="1" ref="F4" ca="1">_xlfn.IFS(D4=1,'Ark1'!$D$2,D4=2, 'Ark1'!$D$3,D4=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1005,19 +1005,19 @@
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xlfn.IFS(D5=1,"CPH",D5=2, "LON",D5=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3" cm="1">
         <f t="array" aca="1" ref="E5" ca="1">_xlfn.IFS(D5=1,'Ark1'!$C$2,D5=2, 'Ark1'!$C$3,D5=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F5" s="3" cm="1">
         <f t="array" aca="1" ref="F5" ca="1">_xlfn.IFS(D5=1,'Ark1'!$D$2,D5=2, 'Ark1'!$D$3,D5=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1029,19 +1029,19 @@
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_xlfn.IFS(D6=1,"CPH",D6=2, "LON",D6=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">_xlfn.IFS(D6=1,'Ark1'!$C$2,D6=2, 'Ark1'!$C$3,D6=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F6" s="3" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">_xlfn.IFS(D6=1,'Ark1'!$D$2,D6=2, 'Ark1'!$D$3,D6=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1061,11 +1061,11 @@
       </c>
       <c r="E7" s="3" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_xlfn.IFS(D7=1,'Ark1'!$C$2,D7=2, 'Ark1'!$C$3,D7=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F7" s="3" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">_xlfn.IFS(D7=1,'Ark1'!$D$2,D7=2, 'Ark1'!$D$3,D7=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1077,19 +1077,19 @@
       </c>
       <c r="C8" t="str" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xlfn.IFS(D8=1,"CPH",D8=2, "LON",D8=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">_xlfn.IFS(D8=1,'Ark1'!$C$2,D8=2, 'Ark1'!$C$3,D8=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F8" s="3" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">_xlfn.IFS(D8=1,'Ark1'!$D$2,D8=2, 'Ark1'!$D$3,D8=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1109,11 +1109,11 @@
       </c>
       <c r="E9" s="3" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xlfn.IFS(D9=1,'Ark1'!$C$2,D9=2, 'Ark1'!$C$3,D9=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F9" s="3" cm="1">
         <f t="array" aca="1" ref="F9" ca="1">_xlfn.IFS(D9=1,'Ark1'!$D$2,D9=2, 'Ark1'!$D$3,D9=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1125,19 +1125,19 @@
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">_xlfn.IFS(D10=1,"CPH",D10=2, "LON",D10=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">_xlfn.IFS(D10=1,'Ark1'!$C$2,D10=2, 'Ark1'!$C$3,D10=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F10" s="3" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">_xlfn.IFS(D10=1,'Ark1'!$D$2,D10=2, 'Ark1'!$D$3,D10=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1149,19 +1149,19 @@
       </c>
       <c r="C11" t="str" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">_xlfn.IFS(D11=1,"CPH",D11=2, "LON",D11=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="3" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">_xlfn.IFS(D11=1,'Ark1'!$C$2,D11=2, 'Ark1'!$C$3,D11=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F11" s="3" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">_xlfn.IFS(D11=1,'Ark1'!$D$2,D11=2, 'Ark1'!$D$3,D11=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1173,19 +1173,19 @@
       </c>
       <c r="C12" t="str" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_xlfn.IFS(D12=1,"CPH",D12=2, "LON",D12=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3" cm="1">
         <f t="array" aca="1" ref="E12" ca="1">_xlfn.IFS(D12=1,'Ark1'!$C$2,D12=2, 'Ark1'!$C$3,D12=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F12" s="3" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">_xlfn.IFS(D12=1,'Ark1'!$D$2,D12=2, 'Ark1'!$D$3,D12=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1197,19 +1197,19 @@
       </c>
       <c r="C13" t="str" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">_xlfn.IFS(D13=1,"CPH",D13=2, "LON",D13=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="3" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">_xlfn.IFS(D13=1,'Ark1'!$C$2,D13=2, 'Ark1'!$C$3,D13=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F13" s="3" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">_xlfn.IFS(D13=1,'Ark1'!$D$2,D13=2, 'Ark1'!$D$3,D13=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1221,19 +1221,19 @@
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">_xlfn.IFS(D14=1,"CPH",D14=2, "LON",D14=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D14">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3" cm="1">
         <f t="array" aca="1" ref="E14" ca="1">_xlfn.IFS(D14=1,'Ark1'!$C$2,D14=2, 'Ark1'!$C$3,D14=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F14" s="3" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">_xlfn.IFS(D14=1,'Ark1'!$D$2,D14=2, 'Ark1'!$D$3,D14=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1245,19 +1245,19 @@
       </c>
       <c r="C15" t="str" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">_xlfn.IFS(D15=1,"CPH",D15=2, "LON",D15=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3" cm="1">
         <f t="array" aca="1" ref="E15" ca="1">_xlfn.IFS(D15=1,'Ark1'!$C$2,D15=2, 'Ark1'!$C$3,D15=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F15" s="3" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">_xlfn.IFS(D15=1,'Ark1'!$D$2,D15=2, 'Ark1'!$D$3,D15=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1277,11 +1277,11 @@
       </c>
       <c r="E16" s="3" cm="1">
         <f t="array" aca="1" ref="E16" ca="1">_xlfn.IFS(D16=1,'Ark1'!$C$2,D16=2, 'Ark1'!$C$3,D16=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F16" s="3" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">_xlfn.IFS(D16=1,'Ark1'!$D$2,D16=2, 'Ark1'!$D$3,D16=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,11 +1301,11 @@
       </c>
       <c r="E17" s="3" cm="1">
         <f t="array" aca="1" ref="E17" ca="1">_xlfn.IFS(D17=1,'Ark1'!$C$2,D17=2, 'Ark1'!$C$3,D17=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F17" s="3" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">_xlfn.IFS(D17=1,'Ark1'!$D$2,D17=2, 'Ark1'!$D$3,D17=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,19 +1317,19 @@
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">_xlfn.IFS(D18=1,"CPH",D18=2, "LON",D18=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="3" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">_xlfn.IFS(D18=1,'Ark1'!$C$2,D18=2, 'Ark1'!$C$3,D18=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F18" s="3" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">_xlfn.IFS(D18=1,'Ark1'!$D$2,D18=2, 'Ark1'!$D$3,D18=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,19 +1341,19 @@
       </c>
       <c r="C19" t="str" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">_xlfn.IFS(D19=1,"CPH",D19=2, "LON",D19=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19" s="3" cm="1">
         <f t="array" aca="1" ref="E19" ca="1">_xlfn.IFS(D19=1,'Ark1'!$C$2,D19=2, 'Ark1'!$C$3,D19=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F19" s="3" cm="1">
         <f t="array" aca="1" ref="F19" ca="1">_xlfn.IFS(D19=1,'Ark1'!$D$2,D19=2, 'Ark1'!$D$3,D19=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1365,19 +1365,19 @@
       </c>
       <c r="C20" t="str" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">_xlfn.IFS(D20=1,"CPH",D20=2, "LON",D20=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3" cm="1">
         <f t="array" aca="1" ref="E20" ca="1">_xlfn.IFS(D20=1,'Ark1'!$C$2,D20=2, 'Ark1'!$C$3,D20=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F20" s="3" cm="1">
         <f t="array" aca="1" ref="F20" ca="1">_xlfn.IFS(D20=1,'Ark1'!$D$2,D20=2, 'Ark1'!$D$3,D20=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,19 +1389,19 @@
       </c>
       <c r="C21" t="str" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">_xlfn.IFS(D21=1,"CPH",D21=2, "LON",D21=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3" cm="1">
         <f t="array" aca="1" ref="E21" ca="1">_xlfn.IFS(D21=1,'Ark1'!$C$2,D21=2, 'Ark1'!$C$3,D21=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F21" s="3" cm="1">
         <f t="array" aca="1" ref="F21" ca="1">_xlfn.IFS(D21=1,'Ark1'!$D$2,D21=2, 'Ark1'!$D$3,D21=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1413,19 +1413,19 @@
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">_xlfn.IFS(D22=1,"CPH",D22=2, "LON",D22=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22" s="3" cm="1">
         <f t="array" aca="1" ref="E22" ca="1">_xlfn.IFS(D22=1,'Ark1'!$C$2,D22=2, 'Ark1'!$C$3,D22=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F22" s="3" cm="1">
         <f t="array" aca="1" ref="F22" ca="1">_xlfn.IFS(D22=1,'Ark1'!$D$2,D22=2, 'Ark1'!$D$3,D22=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1445,11 +1445,11 @@
       </c>
       <c r="E23" s="3" cm="1">
         <f t="array" aca="1" ref="E23" ca="1">_xlfn.IFS(D23=1,'Ark1'!$C$2,D23=2, 'Ark1'!$C$3,D23=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F23" s="3" cm="1">
         <f t="array" aca="1" ref="F23" ca="1">_xlfn.IFS(D23=1,'Ark1'!$D$2,D23=2, 'Ark1'!$D$3,D23=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1469,11 +1469,11 @@
       </c>
       <c r="E24" s="3" cm="1">
         <f t="array" aca="1" ref="E24" ca="1">_xlfn.IFS(D24=1,'Ark1'!$C$2,D24=2, 'Ark1'!$C$3,D24=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F24" s="3" cm="1">
         <f t="array" aca="1" ref="F24" ca="1">_xlfn.IFS(D24=1,'Ark1'!$D$2,D24=2, 'Ark1'!$D$3,D24=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1493,11 +1493,11 @@
       </c>
       <c r="E25" s="3" cm="1">
         <f t="array" aca="1" ref="E25" ca="1">_xlfn.IFS(D25=1,'Ark1'!$C$2,D25=2, 'Ark1'!$C$3,D25=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F25" s="3" cm="1">
         <f t="array" aca="1" ref="F25" ca="1">_xlfn.IFS(D25=1,'Ark1'!$D$2,D25=2, 'Ark1'!$D$3,D25=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="E26" s="3" cm="1">
         <f t="array" aca="1" ref="E26" ca="1">_xlfn.IFS(D26=1,'Ark1'!$C$2,D26=2, 'Ark1'!$C$3,D26=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F26" s="3" cm="1">
         <f t="array" aca="1" ref="F26" ca="1">_xlfn.IFS(D26=1,'Ark1'!$D$2,D26=2, 'Ark1'!$D$3,D26=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1533,19 +1533,19 @@
       </c>
       <c r="C27" t="str" cm="1">
         <f t="array" aca="1" ref="C27" ca="1">_xlfn.IFS(D27=1,"CPH",D27=2, "LON",D27=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3" cm="1">
         <f t="array" aca="1" ref="E27" ca="1">_xlfn.IFS(D27=1,'Ark1'!$C$2,D27=2, 'Ark1'!$C$3,D27=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F27" s="3" cm="1">
         <f t="array" aca="1" ref="F27" ca="1">_xlfn.IFS(D27=1,'Ark1'!$D$2,D27=2, 'Ark1'!$D$3,D27=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1557,19 +1557,19 @@
       </c>
       <c r="C28" t="str" cm="1">
         <f t="array" aca="1" ref="C28" ca="1">_xlfn.IFS(D28=1,"CPH",D28=2, "LON",D28=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="3" cm="1">
         <f t="array" aca="1" ref="E28" ca="1">_xlfn.IFS(D28=1,'Ark1'!$C$2,D28=2, 'Ark1'!$C$3,D28=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F28" s="3" cm="1">
         <f t="array" aca="1" ref="F28" ca="1">_xlfn.IFS(D28=1,'Ark1'!$D$2,D28=2, 'Ark1'!$D$3,D28=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1589,11 +1589,11 @@
       </c>
       <c r="E29" s="3" cm="1">
         <f t="array" aca="1" ref="E29" ca="1">_xlfn.IFS(D29=1,'Ark1'!$C$2,D29=2, 'Ark1'!$C$3,D29=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F29" s="3" cm="1">
         <f t="array" aca="1" ref="F29" ca="1">_xlfn.IFS(D29=1,'Ark1'!$D$2,D29=2, 'Ark1'!$D$3,D29=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1613,11 +1613,11 @@
       </c>
       <c r="E30" s="3" cm="1">
         <f t="array" aca="1" ref="E30" ca="1">_xlfn.IFS(D30=1,'Ark1'!$C$2,D30=2, 'Ark1'!$C$3,D30=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F30" s="3" cm="1">
         <f t="array" aca="1" ref="F30" ca="1">_xlfn.IFS(D30=1,'Ark1'!$D$2,D30=2, 'Ark1'!$D$3,D30=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1629,19 +1629,19 @@
       </c>
       <c r="C31" t="str" cm="1">
         <f t="array" aca="1" ref="C31" ca="1">_xlfn.IFS(D31=1,"CPH",D31=2, "LON",D31=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="3" cm="1">
         <f t="array" aca="1" ref="E31" ca="1">_xlfn.IFS(D31=1,'Ark1'!$C$2,D31=2, 'Ark1'!$C$3,D31=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F31" s="3" cm="1">
         <f t="array" aca="1" ref="F31" ca="1">_xlfn.IFS(D31=1,'Ark1'!$D$2,D31=2, 'Ark1'!$D$3,D31=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1661,11 +1661,11 @@
       </c>
       <c r="E32" s="3" cm="1">
         <f t="array" aca="1" ref="E32" ca="1">_xlfn.IFS(D32=1,'Ark1'!$C$2,D32=2, 'Ark1'!$C$3,D32=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F32" s="3" cm="1">
         <f t="array" aca="1" ref="F32" ca="1">_xlfn.IFS(D32=1,'Ark1'!$D$2,D32=2, 'Ark1'!$D$3,D32=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1677,19 +1677,19 @@
       </c>
       <c r="C33" t="str" cm="1">
         <f t="array" aca="1" ref="C33" ca="1">_xlfn.IFS(D33=1,"CPH",D33=2, "LON",D33=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="3" cm="1">
         <f t="array" aca="1" ref="E33" ca="1">_xlfn.IFS(D33=1,'Ark1'!$C$2,D33=2, 'Ark1'!$C$3,D33=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F33" s="3" cm="1">
         <f t="array" aca="1" ref="F33" ca="1">_xlfn.IFS(D33=1,'Ark1'!$D$2,D33=2, 'Ark1'!$D$3,D33=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1701,19 +1701,19 @@
       </c>
       <c r="C34" t="str" cm="1">
         <f t="array" aca="1" ref="C34" ca="1">_xlfn.IFS(D34=1,"CPH",D34=2, "LON",D34=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E34" s="3" cm="1">
         <f t="array" aca="1" ref="E34" ca="1">_xlfn.IFS(D34=1,'Ark1'!$C$2,D34=2, 'Ark1'!$C$3,D34=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F34" s="3" cm="1">
         <f t="array" aca="1" ref="F34" ca="1">_xlfn.IFS(D34=1,'Ark1'!$D$2,D34=2, 'Ark1'!$D$3,D34=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1733,11 +1733,11 @@
       </c>
       <c r="E35" s="3" cm="1">
         <f t="array" aca="1" ref="E35" ca="1">_xlfn.IFS(D35=1,'Ark1'!$C$2,D35=2, 'Ark1'!$C$3,D35=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F35" s="3" cm="1">
         <f t="array" aca="1" ref="F35" ca="1">_xlfn.IFS(D35=1,'Ark1'!$D$2,D35=2, 'Ark1'!$D$3,D35=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1749,19 +1749,19 @@
       </c>
       <c r="C36" t="str" cm="1">
         <f t="array" aca="1" ref="C36" ca="1">_xlfn.IFS(D36=1,"CPH",D36=2, "LON",D36=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" s="3" cm="1">
         <f t="array" aca="1" ref="E36" ca="1">_xlfn.IFS(D36=1,'Ark1'!$C$2,D36=2, 'Ark1'!$C$3,D36=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F36" s="3" cm="1">
         <f t="array" aca="1" ref="F36" ca="1">_xlfn.IFS(D36=1,'Ark1'!$D$2,D36=2, 'Ark1'!$D$3,D36=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1773,19 +1773,19 @@
       </c>
       <c r="C37" t="str" cm="1">
         <f t="array" aca="1" ref="C37" ca="1">_xlfn.IFS(D37=1,"CPH",D37=2, "LON",D37=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E37" s="3" cm="1">
         <f t="array" aca="1" ref="E37" ca="1">_xlfn.IFS(D37=1,'Ark1'!$C$2,D37=2, 'Ark1'!$C$3,D37=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F37" s="3" cm="1">
         <f t="array" aca="1" ref="F37" ca="1">_xlfn.IFS(D37=1,'Ark1'!$D$2,D37=2, 'Ark1'!$D$3,D37=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1797,19 +1797,19 @@
       </c>
       <c r="C38" t="str" cm="1">
         <f t="array" aca="1" ref="C38" ca="1">_xlfn.IFS(D38=1,"CPH",D38=2, "LON",D38=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="3" cm="1">
         <f t="array" aca="1" ref="E38" ca="1">_xlfn.IFS(D38=1,'Ark1'!$C$2,D38=2, 'Ark1'!$C$3,D38=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F38" s="3" cm="1">
         <f t="array" aca="1" ref="F38" ca="1">_xlfn.IFS(D38=1,'Ark1'!$D$2,D38=2, 'Ark1'!$D$3,D38=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1821,19 +1821,19 @@
       </c>
       <c r="C39" t="str" cm="1">
         <f t="array" aca="1" ref="C39" ca="1">_xlfn.IFS(D39=1,"CPH",D39=2, "LON",D39=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="3" cm="1">
         <f t="array" aca="1" ref="E39" ca="1">_xlfn.IFS(D39=1,'Ark1'!$C$2,D39=2, 'Ark1'!$C$3,D39=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F39" s="3" cm="1">
         <f t="array" aca="1" ref="F39" ca="1">_xlfn.IFS(D39=1,'Ark1'!$D$2,D39=2, 'Ark1'!$D$3,D39=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1845,19 +1845,19 @@
       </c>
       <c r="C40" t="str" cm="1">
         <f t="array" aca="1" ref="C40" ca="1">_xlfn.IFS(D40=1,"CPH",D40=2, "LON",D40=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" s="3" cm="1">
         <f t="array" aca="1" ref="E40" ca="1">_xlfn.IFS(D40=1,'Ark1'!$C$2,D40=2, 'Ark1'!$C$3,D40=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F40" s="3" cm="1">
         <f t="array" aca="1" ref="F40" ca="1">_xlfn.IFS(D40=1,'Ark1'!$D$2,D40=2, 'Ark1'!$D$3,D40=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1877,11 +1877,11 @@
       </c>
       <c r="E41" s="3" cm="1">
         <f t="array" aca="1" ref="E41" ca="1">_xlfn.IFS(D41=1,'Ark1'!$C$2,D41=2, 'Ark1'!$C$3,D41=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F41" s="3" cm="1">
         <f t="array" aca="1" ref="F41" ca="1">_xlfn.IFS(D41=1,'Ark1'!$D$2,D41=2, 'Ark1'!$D$3,D41=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1893,19 +1893,19 @@
       </c>
       <c r="C42" t="str" cm="1">
         <f t="array" aca="1" ref="C42" ca="1">_xlfn.IFS(D42=1,"CPH",D42=2, "LON",D42=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E42" s="3" cm="1">
         <f t="array" aca="1" ref="E42" ca="1">_xlfn.IFS(D42=1,'Ark1'!$C$2,D42=2, 'Ark1'!$C$3,D42=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F42" s="3" cm="1">
         <f t="array" aca="1" ref="F42" ca="1">_xlfn.IFS(D42=1,'Ark1'!$D$2,D42=2, 'Ark1'!$D$3,D42=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,19 +1917,19 @@
       </c>
       <c r="C43" t="str" cm="1">
         <f t="array" aca="1" ref="C43" ca="1">_xlfn.IFS(D43=1,"CPH",D43=2, "LON",D43=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E43" s="3" cm="1">
         <f t="array" aca="1" ref="E43" ca="1">_xlfn.IFS(D43=1,'Ark1'!$C$2,D43=2, 'Ark1'!$C$3,D43=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F43" s="3" cm="1">
         <f t="array" aca="1" ref="F43" ca="1">_xlfn.IFS(D43=1,'Ark1'!$D$2,D43=2, 'Ark1'!$D$3,D43=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1941,19 +1941,19 @@
       </c>
       <c r="C44" t="str" cm="1">
         <f t="array" aca="1" ref="C44" ca="1">_xlfn.IFS(D44=1,"CPH",D44=2, "LON",D44=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="3" cm="1">
         <f t="array" aca="1" ref="E44" ca="1">_xlfn.IFS(D44=1,'Ark1'!$C$2,D44=2, 'Ark1'!$C$3,D44=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F44" s="3" cm="1">
         <f t="array" aca="1" ref="F44" ca="1">_xlfn.IFS(D44=1,'Ark1'!$D$2,D44=2, 'Ark1'!$D$3,D44=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,19 +1965,19 @@
       </c>
       <c r="C45" t="str" cm="1">
         <f t="array" aca="1" ref="C45" ca="1">_xlfn.IFS(D45=1,"CPH",D45=2, "LON",D45=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45" s="3" cm="1">
         <f t="array" aca="1" ref="E45" ca="1">_xlfn.IFS(D45=1,'Ark1'!$C$2,D45=2, 'Ark1'!$C$3,D45=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F45" s="3" cm="1">
         <f t="array" aca="1" ref="F45" ca="1">_xlfn.IFS(D45=1,'Ark1'!$D$2,D45=2, 'Ark1'!$D$3,D45=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1997,11 +1997,11 @@
       </c>
       <c r="E46" s="3" cm="1">
         <f t="array" aca="1" ref="E46" ca="1">_xlfn.IFS(D46=1,'Ark1'!$C$2,D46=2, 'Ark1'!$C$3,D46=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F46" s="3" cm="1">
         <f t="array" aca="1" ref="F46" ca="1">_xlfn.IFS(D46=1,'Ark1'!$D$2,D46=2, 'Ark1'!$D$3,D46=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2021,11 +2021,11 @@
       </c>
       <c r="E47" s="3" cm="1">
         <f t="array" aca="1" ref="E47" ca="1">_xlfn.IFS(D47=1,'Ark1'!$C$2,D47=2, 'Ark1'!$C$3,D47=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F47" s="3" cm="1">
         <f t="array" aca="1" ref="F47" ca="1">_xlfn.IFS(D47=1,'Ark1'!$D$2,D47=2, 'Ark1'!$D$3,D47=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2037,19 +2037,19 @@
       </c>
       <c r="C48" t="str" cm="1">
         <f t="array" aca="1" ref="C48" ca="1">_xlfn.IFS(D48=1,"CPH",D48=2, "LON",D48=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E48" s="3" cm="1">
         <f t="array" aca="1" ref="E48" ca="1">_xlfn.IFS(D48=1,'Ark1'!$C$2,D48=2, 'Ark1'!$C$3,D48=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F48" s="3" cm="1">
         <f t="array" aca="1" ref="F48" ca="1">_xlfn.IFS(D48=1,'Ark1'!$D$2,D48=2, 'Ark1'!$D$3,D48=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2061,19 +2061,19 @@
       </c>
       <c r="C49" t="str" cm="1">
         <f t="array" aca="1" ref="C49" ca="1">_xlfn.IFS(D49=1,"CPH",D49=2, "LON",D49=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E49" s="3" cm="1">
         <f t="array" aca="1" ref="E49" ca="1">_xlfn.IFS(D49=1,'Ark1'!$C$2,D49=2, 'Ark1'!$C$3,D49=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F49" s="3" cm="1">
         <f t="array" aca="1" ref="F49" ca="1">_xlfn.IFS(D49=1,'Ark1'!$D$2,D49=2, 'Ark1'!$D$3,D49=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2093,11 +2093,11 @@
       </c>
       <c r="E50" s="3" cm="1">
         <f t="array" aca="1" ref="E50" ca="1">_xlfn.IFS(D50=1,'Ark1'!$C$2,D50=2, 'Ark1'!$C$3,D50=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F50" s="3" cm="1">
         <f t="array" aca="1" ref="F50" ca="1">_xlfn.IFS(D50=1,'Ark1'!$D$2,D50=2, 'Ark1'!$D$3,D50=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2109,19 +2109,19 @@
       </c>
       <c r="C51" t="str" cm="1">
         <f t="array" aca="1" ref="C51" ca="1">_xlfn.IFS(D51=1,"CPH",D51=2, "LON",D51=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" s="3" cm="1">
         <f t="array" aca="1" ref="E51" ca="1">_xlfn.IFS(D51=1,'Ark1'!$C$2,D51=2, 'Ark1'!$C$3,D51=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F51" s="3" cm="1">
         <f t="array" aca="1" ref="F51" ca="1">_xlfn.IFS(D51=1,'Ark1'!$D$2,D51=2, 'Ark1'!$D$3,D51=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="E52" s="3" cm="1">
         <f t="array" aca="1" ref="E52" ca="1">_xlfn.IFS(D52=1,'Ark1'!$C$2,D52=2, 'Ark1'!$C$3,D52=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F52" s="3" cm="1">
         <f t="array" aca="1" ref="F52" ca="1">_xlfn.IFS(D52=1,'Ark1'!$D$2,D52=2, 'Ark1'!$D$3,D52=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2157,19 +2157,19 @@
       </c>
       <c r="C53" t="str" cm="1">
         <f t="array" aca="1" ref="C53" ca="1">_xlfn.IFS(D53=1,"CPH",D53=2, "LON",D53=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E53" s="3" cm="1">
         <f t="array" aca="1" ref="E53" ca="1">_xlfn.IFS(D53=1,'Ark1'!$C$2,D53=2, 'Ark1'!$C$3,D53=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F53" s="3" cm="1">
         <f t="array" aca="1" ref="F53" ca="1">_xlfn.IFS(D53=1,'Ark1'!$D$2,D53=2, 'Ark1'!$D$3,D53=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2189,11 +2189,11 @@
       </c>
       <c r="E54" s="3" cm="1">
         <f t="array" aca="1" ref="E54" ca="1">_xlfn.IFS(D54=1,'Ark1'!$C$2,D54=2, 'Ark1'!$C$3,D54=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F54" s="3" cm="1">
         <f t="array" aca="1" ref="F54" ca="1">_xlfn.IFS(D54=1,'Ark1'!$D$2,D54=2, 'Ark1'!$D$3,D54=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2205,19 +2205,19 @@
       </c>
       <c r="C55" t="str" cm="1">
         <f t="array" aca="1" ref="C55" ca="1">_xlfn.IFS(D55=1,"CPH",D55=2, "LON",D55=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E55" s="3" cm="1">
         <f t="array" aca="1" ref="E55" ca="1">_xlfn.IFS(D55=1,'Ark1'!$C$2,D55=2, 'Ark1'!$C$3,D55=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F55" s="3" cm="1">
         <f t="array" aca="1" ref="F55" ca="1">_xlfn.IFS(D55=1,'Ark1'!$D$2,D55=2, 'Ark1'!$D$3,D55=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2237,11 +2237,11 @@
       </c>
       <c r="E56" s="3" cm="1">
         <f t="array" aca="1" ref="E56" ca="1">_xlfn.IFS(D56=1,'Ark1'!$C$2,D56=2, 'Ark1'!$C$3,D56=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F56" s="3" cm="1">
         <f t="array" aca="1" ref="F56" ca="1">_xlfn.IFS(D56=1,'Ark1'!$D$2,D56=2, 'Ark1'!$D$3,D56=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2253,19 +2253,19 @@
       </c>
       <c r="C57" t="str" cm="1">
         <f t="array" aca="1" ref="C57" ca="1">_xlfn.IFS(D57=1,"CPH",D57=2, "LON",D57=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57" s="3" cm="1">
         <f t="array" aca="1" ref="E57" ca="1">_xlfn.IFS(D57=1,'Ark1'!$C$2,D57=2, 'Ark1'!$C$3,D57=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F57" s="3" cm="1">
         <f t="array" aca="1" ref="F57" ca="1">_xlfn.IFS(D57=1,'Ark1'!$D$2,D57=2, 'Ark1'!$D$3,D57=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2277,19 +2277,19 @@
       </c>
       <c r="C58" t="str" cm="1">
         <f t="array" aca="1" ref="C58" ca="1">_xlfn.IFS(D58=1,"CPH",D58=2, "LON",D58=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E58" s="3" cm="1">
         <f t="array" aca="1" ref="E58" ca="1">_xlfn.IFS(D58=1,'Ark1'!$C$2,D58=2, 'Ark1'!$C$3,D58=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F58" s="3" cm="1">
         <f t="array" aca="1" ref="F58" ca="1">_xlfn.IFS(D58=1,'Ark1'!$D$2,D58=2, 'Ark1'!$D$3,D58=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2301,19 +2301,19 @@
       </c>
       <c r="C59" t="str" cm="1">
         <f t="array" aca="1" ref="C59" ca="1">_xlfn.IFS(D59=1,"CPH",D59=2, "LON",D59=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E59" s="3" cm="1">
         <f t="array" aca="1" ref="E59" ca="1">_xlfn.IFS(D59=1,'Ark1'!$C$2,D59=2, 'Ark1'!$C$3,D59=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F59" s="3" cm="1">
         <f t="array" aca="1" ref="F59" ca="1">_xlfn.IFS(D59=1,'Ark1'!$D$2,D59=2, 'Ark1'!$D$3,D59=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2325,19 +2325,19 @@
       </c>
       <c r="C60" t="str" cm="1">
         <f t="array" aca="1" ref="C60" ca="1">_xlfn.IFS(D60=1,"CPH",D60=2, "LON",D60=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" s="3" cm="1">
         <f t="array" aca="1" ref="E60" ca="1">_xlfn.IFS(D60=1,'Ark1'!$C$2,D60=2, 'Ark1'!$C$3,D60=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F60" s="3" cm="1">
         <f t="array" aca="1" ref="F60" ca="1">_xlfn.IFS(D60=1,'Ark1'!$D$2,D60=2, 'Ark1'!$D$3,D60=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2349,19 +2349,19 @@
       </c>
       <c r="C61" t="str" cm="1">
         <f t="array" aca="1" ref="C61" ca="1">_xlfn.IFS(D61=1,"CPH",D61=2, "LON",D61=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E61" s="3" cm="1">
         <f t="array" aca="1" ref="E61" ca="1">_xlfn.IFS(D61=1,'Ark1'!$C$2,D61=2, 'Ark1'!$C$3,D61=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F61" s="3" cm="1">
         <f t="array" aca="1" ref="F61" ca="1">_xlfn.IFS(D61=1,'Ark1'!$D$2,D61=2, 'Ark1'!$D$3,D61=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2381,11 +2381,11 @@
       </c>
       <c r="E62" s="3" cm="1">
         <f t="array" aca="1" ref="E62" ca="1">_xlfn.IFS(D62=1,'Ark1'!$C$2,D62=2, 'Ark1'!$C$3,D62=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F62" s="3" cm="1">
         <f t="array" aca="1" ref="F62" ca="1">_xlfn.IFS(D62=1,'Ark1'!$D$2,D62=2, 'Ark1'!$D$3,D62=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2397,19 +2397,19 @@
       </c>
       <c r="C63" t="str" cm="1">
         <f t="array" aca="1" ref="C63" ca="1">_xlfn.IFS(D63=1,"CPH",D63=2, "LON",D63=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" s="3" cm="1">
         <f t="array" aca="1" ref="E63" ca="1">_xlfn.IFS(D63=1,'Ark1'!$C$2,D63=2, 'Ark1'!$C$3,D63=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F63" s="3" cm="1">
         <f t="array" aca="1" ref="F63" ca="1">_xlfn.IFS(D63=1,'Ark1'!$D$2,D63=2, 'Ark1'!$D$3,D63=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2421,19 +2421,19 @@
       </c>
       <c r="C64" t="str" cm="1">
         <f t="array" aca="1" ref="C64" ca="1">_xlfn.IFS(D64=1,"CPH",D64=2, "LON",D64=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E64" s="3" cm="1">
         <f t="array" aca="1" ref="E64" ca="1">_xlfn.IFS(D64=1,'Ark1'!$C$2,D64=2, 'Ark1'!$C$3,D64=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F64" s="3" cm="1">
         <f t="array" aca="1" ref="F64" ca="1">_xlfn.IFS(D64=1,'Ark1'!$D$2,D64=2, 'Ark1'!$D$3,D64=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2445,19 +2445,19 @@
       </c>
       <c r="C65" t="str" cm="1">
         <f t="array" aca="1" ref="C65" ca="1">_xlfn.IFS(D65=1,"CPH",D65=2, "LON",D65=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E65" s="3" cm="1">
         <f t="array" aca="1" ref="E65" ca="1">_xlfn.IFS(D65=1,'Ark1'!$C$2,D65=2, 'Ark1'!$C$3,D65=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F65" s="3" cm="1">
         <f t="array" aca="1" ref="F65" ca="1">_xlfn.IFS(D65=1,'Ark1'!$D$2,D65=2, 'Ark1'!$D$3,D65=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,19 +2469,19 @@
       </c>
       <c r="C66" t="str" cm="1">
         <f t="array" aca="1" ref="C66" ca="1">_xlfn.IFS(D66=1,"CPH",D66=2, "LON",D66=3,"STO")</f>
-        <v>CPH</v>
+        <v>STO</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E66" s="3" cm="1">
         <f t="array" aca="1" ref="E66" ca="1">_xlfn.IFS(D66=1,'Ark1'!$C$2,D66=2, 'Ark1'!$C$3,D66=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F66" s="3" cm="1">
         <f t="array" aca="1" ref="F66" ca="1">_xlfn.IFS(D66=1,'Ark1'!$D$2,D66=2, 'Ark1'!$D$3,D66=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2493,19 +2493,19 @@
       </c>
       <c r="C67" t="str" cm="1">
         <f t="array" aca="1" ref="C67" ca="1">_xlfn.IFS(D67=1,"CPH",D67=2, "LON",D67=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D67">
         <f t="shared" ref="D67:D101" ca="1" si="1">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67" s="3" cm="1">
         <f t="array" aca="1" ref="E67" ca="1">_xlfn.IFS(D67=1,'Ark1'!$C$2,D67=2, 'Ark1'!$C$3,D67=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F67" s="3" cm="1">
         <f t="array" aca="1" ref="F67" ca="1">_xlfn.IFS(D67=1,'Ark1'!$D$2,D67=2, 'Ark1'!$D$3,D67=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2525,11 +2525,11 @@
       </c>
       <c r="E68" s="3" cm="1">
         <f t="array" aca="1" ref="E68" ca="1">_xlfn.IFS(D68=1,'Ark1'!$C$2,D68=2, 'Ark1'!$C$3,D68=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F68" s="3" cm="1">
         <f t="array" aca="1" ref="F68" ca="1">_xlfn.IFS(D68=1,'Ark1'!$D$2,D68=2, 'Ark1'!$D$3,D68=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2541,19 +2541,19 @@
       </c>
       <c r="C69" t="str" cm="1">
         <f t="array" aca="1" ref="C69" ca="1">_xlfn.IFS(D69=1,"CPH",D69=2, "LON",D69=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E69" s="3" cm="1">
         <f t="array" aca="1" ref="E69" ca="1">_xlfn.IFS(D69=1,'Ark1'!$C$2,D69=2, 'Ark1'!$C$3,D69=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F69" s="3" cm="1">
         <f t="array" aca="1" ref="F69" ca="1">_xlfn.IFS(D69=1,'Ark1'!$D$2,D69=2, 'Ark1'!$D$3,D69=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2565,19 +2565,19 @@
       </c>
       <c r="C70" t="str" cm="1">
         <f t="array" aca="1" ref="C70" ca="1">_xlfn.IFS(D70=1,"CPH",D70=2, "LON",D70=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70" s="3" cm="1">
         <f t="array" aca="1" ref="E70" ca="1">_xlfn.IFS(D70=1,'Ark1'!$C$2,D70=2, 'Ark1'!$C$3,D70=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F70" s="3" cm="1">
         <f t="array" aca="1" ref="F70" ca="1">_xlfn.IFS(D70=1,'Ark1'!$D$2,D70=2, 'Ark1'!$D$3,D70=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2589,19 +2589,19 @@
       </c>
       <c r="C71" t="str" cm="1">
         <f t="array" aca="1" ref="C71" ca="1">_xlfn.IFS(D71=1,"CPH",D71=2, "LON",D71=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E71" s="3" cm="1">
         <f t="array" aca="1" ref="E71" ca="1">_xlfn.IFS(D71=1,'Ark1'!$C$2,D71=2, 'Ark1'!$C$3,D71=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F71" s="3" cm="1">
         <f t="array" aca="1" ref="F71" ca="1">_xlfn.IFS(D71=1,'Ark1'!$D$2,D71=2, 'Ark1'!$D$3,D71=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2613,19 +2613,19 @@
       </c>
       <c r="C72" t="str" cm="1">
         <f t="array" aca="1" ref="C72" ca="1">_xlfn.IFS(D72=1,"CPH",D72=2, "LON",D72=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E72" s="3" cm="1">
         <f t="array" aca="1" ref="E72" ca="1">_xlfn.IFS(D72=1,'Ark1'!$C$2,D72=2, 'Ark1'!$C$3,D72=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F72" s="3" cm="1">
         <f t="array" aca="1" ref="F72" ca="1">_xlfn.IFS(D72=1,'Ark1'!$D$2,D72=2, 'Ark1'!$D$3,D72=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2637,19 +2637,19 @@
       </c>
       <c r="C73" t="str" cm="1">
         <f t="array" aca="1" ref="C73" ca="1">_xlfn.IFS(D73=1,"CPH",D73=2, "LON",D73=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E73" s="3" cm="1">
         <f t="array" aca="1" ref="E73" ca="1">_xlfn.IFS(D73=1,'Ark1'!$C$2,D73=2, 'Ark1'!$C$3,D73=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F73" s="3" cm="1">
         <f t="array" aca="1" ref="F73" ca="1">_xlfn.IFS(D73=1,'Ark1'!$D$2,D73=2, 'Ark1'!$D$3,D73=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2669,11 +2669,11 @@
       </c>
       <c r="E74" s="3" cm="1">
         <f t="array" aca="1" ref="E74" ca="1">_xlfn.IFS(D74=1,'Ark1'!$C$2,D74=2, 'Ark1'!$C$3,D74=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F74" s="3" cm="1">
         <f t="array" aca="1" ref="F74" ca="1">_xlfn.IFS(D74=1,'Ark1'!$D$2,D74=2, 'Ark1'!$D$3,D74=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2685,19 +2685,19 @@
       </c>
       <c r="C75" t="str" cm="1">
         <f t="array" aca="1" ref="C75" ca="1">_xlfn.IFS(D75=1,"CPH",D75=2, "LON",D75=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E75" s="3" cm="1">
         <f t="array" aca="1" ref="E75" ca="1">_xlfn.IFS(D75=1,'Ark1'!$C$2,D75=2, 'Ark1'!$C$3,D75=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F75" s="3" cm="1">
         <f t="array" aca="1" ref="F75" ca="1">_xlfn.IFS(D75=1,'Ark1'!$D$2,D75=2, 'Ark1'!$D$3,D75=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2717,11 +2717,11 @@
       </c>
       <c r="E76" s="3" cm="1">
         <f t="array" aca="1" ref="E76" ca="1">_xlfn.IFS(D76=1,'Ark1'!$C$2,D76=2, 'Ark1'!$C$3,D76=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F76" s="3" cm="1">
         <f t="array" aca="1" ref="F76" ca="1">_xlfn.IFS(D76=1,'Ark1'!$D$2,D76=2, 'Ark1'!$D$3,D76=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2741,11 +2741,11 @@
       </c>
       <c r="E77" s="3" cm="1">
         <f t="array" aca="1" ref="E77" ca="1">_xlfn.IFS(D77=1,'Ark1'!$C$2,D77=2, 'Ark1'!$C$3,D77=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F77" s="3" cm="1">
         <f t="array" aca="1" ref="F77" ca="1">_xlfn.IFS(D77=1,'Ark1'!$D$2,D77=2, 'Ark1'!$D$3,D77=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2765,11 +2765,11 @@
       </c>
       <c r="E78" s="3" cm="1">
         <f t="array" aca="1" ref="E78" ca="1">_xlfn.IFS(D78=1,'Ark1'!$C$2,D78=2, 'Ark1'!$C$3,D78=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F78" s="3" cm="1">
         <f t="array" aca="1" ref="F78" ca="1">_xlfn.IFS(D78=1,'Ark1'!$D$2,D78=2, 'Ark1'!$D$3,D78=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2781,19 +2781,19 @@
       </c>
       <c r="C79" t="str" cm="1">
         <f t="array" aca="1" ref="C79" ca="1">_xlfn.IFS(D79=1,"CPH",D79=2, "LON",D79=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E79" s="3" cm="1">
         <f t="array" aca="1" ref="E79" ca="1">_xlfn.IFS(D79=1,'Ark1'!$C$2,D79=2, 'Ark1'!$C$3,D79=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F79" s="3" cm="1">
         <f t="array" aca="1" ref="F79" ca="1">_xlfn.IFS(D79=1,'Ark1'!$D$2,D79=2, 'Ark1'!$D$3,D79=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2805,19 +2805,19 @@
       </c>
       <c r="C80" t="str" cm="1">
         <f t="array" aca="1" ref="C80" ca="1">_xlfn.IFS(D80=1,"CPH",D80=2, "LON",D80=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E80" s="3" cm="1">
         <f t="array" aca="1" ref="E80" ca="1">_xlfn.IFS(D80=1,'Ark1'!$C$2,D80=2, 'Ark1'!$C$3,D80=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F80" s="3" cm="1">
         <f t="array" aca="1" ref="F80" ca="1">_xlfn.IFS(D80=1,'Ark1'!$D$2,D80=2, 'Ark1'!$D$3,D80=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2829,19 +2829,19 @@
       </c>
       <c r="C81" t="str" cm="1">
         <f t="array" aca="1" ref="C81" ca="1">_xlfn.IFS(D81=1,"CPH",D81=2, "LON",D81=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E81" s="3" cm="1">
         <f t="array" aca="1" ref="E81" ca="1">_xlfn.IFS(D81=1,'Ark1'!$C$2,D81=2, 'Ark1'!$C$3,D81=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F81" s="3" cm="1">
         <f t="array" aca="1" ref="F81" ca="1">_xlfn.IFS(D81=1,'Ark1'!$D$2,D81=2, 'Ark1'!$D$3,D81=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2853,19 +2853,19 @@
       </c>
       <c r="C82" t="str" cm="1">
         <f t="array" aca="1" ref="C82" ca="1">_xlfn.IFS(D82=1,"CPH",D82=2, "LON",D82=3,"STO")</f>
-        <v>LON</v>
+        <v>CPH</v>
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E82" s="3" cm="1">
         <f t="array" aca="1" ref="E82" ca="1">_xlfn.IFS(D82=1,'Ark1'!$C$2,D82=2, 'Ark1'!$C$3,D82=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F82" s="3" cm="1">
         <f t="array" aca="1" ref="F82" ca="1">_xlfn.IFS(D82=1,'Ark1'!$D$2,D82=2, 'Ark1'!$D$3,D82=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2877,19 +2877,19 @@
       </c>
       <c r="C83" t="str" cm="1">
         <f t="array" aca="1" ref="C83" ca="1">_xlfn.IFS(D83=1,"CPH",D83=2, "LON",D83=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E83" s="3" cm="1">
         <f t="array" aca="1" ref="E83" ca="1">_xlfn.IFS(D83=1,'Ark1'!$C$2,D83=2, 'Ark1'!$C$3,D83=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F83" s="3" cm="1">
         <f t="array" aca="1" ref="F83" ca="1">_xlfn.IFS(D83=1,'Ark1'!$D$2,D83=2, 'Ark1'!$D$3,D83=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2901,19 +2901,19 @@
       </c>
       <c r="C84" t="str" cm="1">
         <f t="array" aca="1" ref="C84" ca="1">_xlfn.IFS(D84=1,"CPH",D84=2, "LON",D84=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E84" s="3" cm="1">
         <f t="array" aca="1" ref="E84" ca="1">_xlfn.IFS(D84=1,'Ark1'!$C$2,D84=2, 'Ark1'!$C$3,D84=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F84" s="3" cm="1">
         <f t="array" aca="1" ref="F84" ca="1">_xlfn.IFS(D84=1,'Ark1'!$D$2,D84=2, 'Ark1'!$D$3,D84=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2925,19 +2925,19 @@
       </c>
       <c r="C85" t="str" cm="1">
         <f t="array" aca="1" ref="C85" ca="1">_xlfn.IFS(D85=1,"CPH",D85=2, "LON",D85=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E85" s="3" cm="1">
         <f t="array" aca="1" ref="E85" ca="1">_xlfn.IFS(D85=1,'Ark1'!$C$2,D85=2, 'Ark1'!$C$3,D85=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F85" s="3" cm="1">
         <f t="array" aca="1" ref="F85" ca="1">_xlfn.IFS(D85=1,'Ark1'!$D$2,D85=2, 'Ark1'!$D$3,D85=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2949,19 +2949,19 @@
       </c>
       <c r="C86" t="str" cm="1">
         <f t="array" aca="1" ref="C86" ca="1">_xlfn.IFS(D86=1,"CPH",D86=2, "LON",D86=3,"STO")</f>
-        <v>LON</v>
+        <v>STO</v>
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E86" s="3" cm="1">
         <f t="array" aca="1" ref="E86" ca="1">_xlfn.IFS(D86=1,'Ark1'!$C$2,D86=2, 'Ark1'!$C$3,D86=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F86" s="3" cm="1">
         <f t="array" aca="1" ref="F86" ca="1">_xlfn.IFS(D86=1,'Ark1'!$D$2,D86=2, 'Ark1'!$D$3,D86=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2973,19 +2973,19 @@
       </c>
       <c r="C87" t="str" cm="1">
         <f t="array" aca="1" ref="C87" ca="1">_xlfn.IFS(D87=1,"CPH",D87=2, "LON",D87=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E87" s="3" cm="1">
         <f t="array" aca="1" ref="E87" ca="1">_xlfn.IFS(D87=1,'Ark1'!$C$2,D87=2, 'Ark1'!$C$3,D87=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F87" s="3" cm="1">
         <f t="array" aca="1" ref="F87" ca="1">_xlfn.IFS(D87=1,'Ark1'!$D$2,D87=2, 'Ark1'!$D$3,D87=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2997,19 +2997,19 @@
       </c>
       <c r="C88" t="str" cm="1">
         <f t="array" aca="1" ref="C88" ca="1">_xlfn.IFS(D88=1,"CPH",D88=2, "LON",D88=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E88" s="3" cm="1">
         <f t="array" aca="1" ref="E88" ca="1">_xlfn.IFS(D88=1,'Ark1'!$C$2,D88=2, 'Ark1'!$C$3,D88=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F88" s="3" cm="1">
         <f t="array" aca="1" ref="F88" ca="1">_xlfn.IFS(D88=1,'Ark1'!$D$2,D88=2, 'Ark1'!$D$3,D88=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3029,11 +3029,11 @@
       </c>
       <c r="E89" s="3" cm="1">
         <f t="array" aca="1" ref="E89" ca="1">_xlfn.IFS(D89=1,'Ark1'!$C$2,D89=2, 'Ark1'!$C$3,D89=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F89" s="3" cm="1">
         <f t="array" aca="1" ref="F89" ca="1">_xlfn.IFS(D89=1,'Ark1'!$D$2,D89=2, 'Ark1'!$D$3,D89=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3045,19 +3045,19 @@
       </c>
       <c r="C90" t="str" cm="1">
         <f t="array" aca="1" ref="C90" ca="1">_xlfn.IFS(D90=1,"CPH",D90=2, "LON",D90=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E90" s="3" cm="1">
         <f t="array" aca="1" ref="E90" ca="1">_xlfn.IFS(D90=1,'Ark1'!$C$2,D90=2, 'Ark1'!$C$3,D90=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F90" s="3" cm="1">
         <f t="array" aca="1" ref="F90" ca="1">_xlfn.IFS(D90=1,'Ark1'!$D$2,D90=2, 'Ark1'!$D$3,D90=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3069,19 +3069,19 @@
       </c>
       <c r="C91" t="str" cm="1">
         <f t="array" aca="1" ref="C91" ca="1">_xlfn.IFS(D91=1,"CPH",D91=2, "LON",D91=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E91" s="3" cm="1">
         <f t="array" aca="1" ref="E91" ca="1">_xlfn.IFS(D91=1,'Ark1'!$C$2,D91=2, 'Ark1'!$C$3,D91=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F91" s="3" cm="1">
         <f t="array" aca="1" ref="F91" ca="1">_xlfn.IFS(D91=1,'Ark1'!$D$2,D91=2, 'Ark1'!$D$3,D91=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3093,19 +3093,19 @@
       </c>
       <c r="C92" t="str" cm="1">
         <f t="array" aca="1" ref="C92" ca="1">_xlfn.IFS(D92=1,"CPH",D92=2, "LON",D92=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E92" s="3" cm="1">
         <f t="array" aca="1" ref="E92" ca="1">_xlfn.IFS(D92=1,'Ark1'!$C$2,D92=2, 'Ark1'!$C$3,D92=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F92" s="3" cm="1">
         <f t="array" aca="1" ref="F92" ca="1">_xlfn.IFS(D92=1,'Ark1'!$D$2,D92=2, 'Ark1'!$D$3,D92=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3117,19 +3117,19 @@
       </c>
       <c r="C93" t="str" cm="1">
         <f t="array" aca="1" ref="C93" ca="1">_xlfn.IFS(D93=1,"CPH",D93=2, "LON",D93=3,"STO")</f>
-        <v>STO</v>
+        <v>LON</v>
       </c>
       <c r="D93">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E93" s="3" cm="1">
         <f t="array" aca="1" ref="E93" ca="1">_xlfn.IFS(D93=1,'Ark1'!$C$2,D93=2, 'Ark1'!$C$3,D93=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F93" s="3" cm="1">
         <f t="array" aca="1" ref="F93" ca="1">_xlfn.IFS(D93=1,'Ark1'!$D$2,D93=2, 'Ark1'!$D$3,D93=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3149,11 +3149,11 @@
       </c>
       <c r="E94" s="3" cm="1">
         <f t="array" aca="1" ref="E94" ca="1">_xlfn.IFS(D94=1,'Ark1'!$C$2,D94=2, 'Ark1'!$C$3,D94=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F94" s="3" cm="1">
         <f t="array" aca="1" ref="F94" ca="1">_xlfn.IFS(D94=1,'Ark1'!$D$2,D94=2, 'Ark1'!$D$3,D94=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3165,19 +3165,19 @@
       </c>
       <c r="C95" t="str" cm="1">
         <f t="array" aca="1" ref="C95" ca="1">_xlfn.IFS(D95=1,"CPH",D95=2, "LON",D95=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E95" s="3" cm="1">
         <f t="array" aca="1" ref="E95" ca="1">_xlfn.IFS(D95=1,'Ark1'!$C$2,D95=2, 'Ark1'!$C$3,D95=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F95" s="3" cm="1">
         <f t="array" aca="1" ref="F95" ca="1">_xlfn.IFS(D95=1,'Ark1'!$D$2,D95=2, 'Ark1'!$D$3,D95=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3189,19 +3189,19 @@
       </c>
       <c r="C96" t="str" cm="1">
         <f t="array" aca="1" ref="C96" ca="1">_xlfn.IFS(D96=1,"CPH",D96=2, "LON",D96=3,"STO")</f>
-        <v>STO</v>
+        <v>CPH</v>
       </c>
       <c r="D96">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E96" s="3" cm="1">
         <f t="array" aca="1" ref="E96" ca="1">_xlfn.IFS(D96=1,'Ark1'!$C$2,D96=2, 'Ark1'!$C$3,D96=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F96" s="3" cm="1">
         <f t="array" aca="1" ref="F96" ca="1">_xlfn.IFS(D96=1,'Ark1'!$D$2,D96=2, 'Ark1'!$D$3,D96=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3221,11 +3221,11 @@
       </c>
       <c r="E97" s="3" cm="1">
         <f t="array" aca="1" ref="E97" ca="1">_xlfn.IFS(D97=1,'Ark1'!$C$2,D97=2, 'Ark1'!$C$3,D97=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F97" s="3" cm="1">
         <f t="array" aca="1" ref="F97" ca="1">_xlfn.IFS(D97=1,'Ark1'!$D$2,D97=2, 'Ark1'!$D$3,D97=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.391734375</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3237,19 +3237,19 @@
       </c>
       <c r="C98" t="str" cm="1">
         <f t="array" aca="1" ref="C98" ca="1">_xlfn.IFS(D98=1,"CPH",D98=2, "LON",D98=3,"STO")</f>
-        <v>CPH</v>
+        <v>LON</v>
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E98" s="3" cm="1">
         <f t="array" aca="1" ref="E98" ca="1">_xlfn.IFS(D98=1,'Ark1'!$C$2,D98=2, 'Ark1'!$C$3,D98=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F98" s="3" cm="1">
         <f t="array" aca="1" ref="F98" ca="1">_xlfn.IFS(D98=1,'Ark1'!$D$2,D98=2, 'Ark1'!$D$3,D98=3,'Ark1'!$D$4)</f>
-        <v>44263.759250347219</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3269,11 +3269,11 @@
       </c>
       <c r="E99" s="3" cm="1">
         <f t="array" aca="1" ref="E99" ca="1">_xlfn.IFS(D99=1,'Ark1'!$C$2,D99=2, 'Ark1'!$C$3,D99=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F99" s="3" cm="1">
         <f t="array" aca="1" ref="F99" ca="1">_xlfn.IFS(D99=1,'Ark1'!$D$2,D99=2, 'Ark1'!$D$3,D99=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3293,11 +3293,11 @@
       </c>
       <c r="E100" s="3" cm="1">
         <f t="array" aca="1" ref="E100" ca="1">_xlfn.IFS(D100=1,'Ark1'!$C$2,D100=2, 'Ark1'!$C$3,D100=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F100" s="3" cm="1">
         <f t="array" aca="1" ref="F100" ca="1">_xlfn.IFS(D100=1,'Ark1'!$D$2,D100=2, 'Ark1'!$D$3,D100=3,'Ark1'!$D$4)</f>
-        <v>44263.759944791665</v>
+        <v>44264.392428819447</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3317,11 +3317,11 @@
       </c>
       <c r="E101" s="3" cm="1">
         <f t="array" aca="1" ref="E101" ca="1">_xlfn.IFS(D101=1,'Ark1'!$C$2,D101=2, 'Ark1'!$C$3,D101=3,'Ark1'!$C$4)</f>
-        <v>44263.757167013886</v>
+        <v>44264.389651041667</v>
       </c>
       <c r="F101" s="3" cm="1">
         <f t="array" aca="1" ref="F101" ca="1">_xlfn.IFS(D101=1,'Ark1'!$D$2,D101=2, 'Ark1'!$D$3,D101=3,'Ark1'!$D$4)</f>
-        <v>44263.760639236105</v>
+        <v>44264.393123263886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>